<commit_message>
ammo system visualized and add leaf map collision with brick almost complete
</commit_message>
<xml_diff>
--- a/map_layout.xlsx
+++ b/map_layout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>=</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>S</t>
-  </si>
-  <si>
-    <t>P=256,1536</t>
   </si>
 </sst>
 </file>
@@ -59,7 +56,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +105,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -121,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -142,6 +145,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:BB93"/>
+  <dimension ref="C1:CO120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="Y64" workbookViewId="0">
+      <selection activeCell="F86" sqref="F64:BY86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -463,13 +474,13 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="S2" s="10"/>
     </row>
     <row r="3" spans="4:45" x14ac:dyDescent="0.2">
@@ -477,13 +488,13 @@
       <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
       <c r="S3" s="11"/>
     </row>
     <row r="4" spans="4:45" x14ac:dyDescent="0.2">
@@ -493,16 +504,16 @@
       <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
       <c r="S4" s="9"/>
     </row>
     <row r="5" spans="4:45" x14ac:dyDescent="0.2">
@@ -512,13 +523,13 @@
       <c r="E5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
     </row>
     <row r="7" spans="4:45" x14ac:dyDescent="0.2">
       <c r="AI7" s="3"/>
@@ -678,12 +689,12 @@
       <c r="AN16" s="1"/>
     </row>
     <row r="17" spans="3:47" x14ac:dyDescent="0.2">
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
       <c r="L17" s="1"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
@@ -693,12 +704,12 @@
       <c r="AN17" s="1"/>
     </row>
     <row r="18" spans="3:47" x14ac:dyDescent="0.2">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
       <c r="L18" s="1"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
@@ -708,12 +719,12 @@
       <c r="AN18" s="1"/>
     </row>
     <row r="19" spans="3:47" x14ac:dyDescent="0.2">
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="L19" s="1"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="1"/>
@@ -730,12 +741,12 @@
       <c r="AN19" s="1"/>
     </row>
     <row r="20" spans="3:47" x14ac:dyDescent="0.2">
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="L20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="3"/>
@@ -1241,7 +1252,54 @@
     <row r="46" spans="12:47" x14ac:dyDescent="0.2">
       <c r="AI46" s="3"/>
     </row>
-    <row r="62" spans="25:39" x14ac:dyDescent="0.2">
+    <row r="57" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="Z57" s="3"/>
+      <c r="AA57" s="3"/>
+      <c r="AB57" s="3"/>
+      <c r="AC57" s="3"/>
+      <c r="AD57" s="3"/>
+      <c r="AE57" s="3"/>
+    </row>
+    <row r="58" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="Z58" s="3"/>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="3"/>
+      <c r="AC58" s="3"/>
+      <c r="AD58" s="3"/>
+      <c r="AE58" s="3"/>
+    </row>
+    <row r="59" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="Z59" s="3"/>
+      <c r="AA59" s="3"/>
+      <c r="AB59" s="3"/>
+      <c r="AC59" s="3"/>
+      <c r="AD59" s="3"/>
+      <c r="AE59" s="3"/>
+    </row>
+    <row r="60" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="Z60" s="3"/>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="3"/>
+      <c r="AC60" s="3"/>
+      <c r="AD60" s="3"/>
+      <c r="AE60" s="3"/>
+    </row>
+    <row r="61" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="Z61" s="3"/>
+      <c r="AA61" s="3"/>
+      <c r="AB61" s="3"/>
+      <c r="AC61" s="3"/>
+      <c r="AD61" s="3"/>
+      <c r="AE61" s="3"/>
+      <c r="BR61" s="3"/>
+      <c r="BS61" s="3"/>
+      <c r="BT61" s="3"/>
+      <c r="BU61" s="3"/>
+      <c r="BV61" s="3"/>
+      <c r="BW61" s="3"/>
+      <c r="BX61" s="3"/>
+    </row>
+    <row r="62" spans="6:76" x14ac:dyDescent="0.2">
       <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
       <c r="AA62" s="3"/>
@@ -1257,8 +1315,19 @@
       <c r="AK62" s="3"/>
       <c r="AL62" s="3"/>
       <c r="AM62" s="3"/>
-    </row>
-    <row r="63" spans="25:39" x14ac:dyDescent="0.2">
+      <c r="BR62" s="3"/>
+      <c r="BS62" s="3"/>
+      <c r="BT62" s="3"/>
+      <c r="BU62" s="3"/>
+      <c r="BV62" s="3"/>
+      <c r="BW62" s="3"/>
+      <c r="BX62" s="3"/>
+    </row>
+    <row r="63" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
       <c r="AA63" s="3"/>
@@ -1274,8 +1343,19 @@
       <c r="AK63" s="3"/>
       <c r="AL63" s="3"/>
       <c r="AM63" s="3"/>
-    </row>
-    <row r="64" spans="25:39" x14ac:dyDescent="0.2">
+      <c r="BR63" s="3"/>
+      <c r="BS63" s="3"/>
+      <c r="BT63" s="3"/>
+      <c r="BU63" s="3"/>
+      <c r="BV63" s="3"/>
+      <c r="BW63" s="3"/>
+      <c r="BX63" s="3"/>
+    </row>
+    <row r="64" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
       <c r="Y64" s="3"/>
       <c r="Z64" s="3"/>
       <c r="AA64" s="3"/>
@@ -1291,8 +1371,19 @@
       <c r="AK64" s="3"/>
       <c r="AL64" s="3"/>
       <c r="AM64" s="3"/>
-    </row>
-    <row r="65" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="BR64" s="3"/>
+      <c r="BS64" s="3"/>
+      <c r="BT64" s="3"/>
+      <c r="BU64" s="3"/>
+      <c r="BV64" s="3"/>
+      <c r="BW64" s="3"/>
+      <c r="BX64" s="3"/>
+    </row>
+    <row r="65" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
       <c r="R65" s="3"/>
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
@@ -1322,298 +1413,516 @@
       <c r="AR65" s="3"/>
       <c r="AS65" s="3"/>
       <c r="AT65" s="3"/>
-    </row>
-    <row r="66" spans="15:54" x14ac:dyDescent="0.2">
-      <c r="R66" s="3"/>
-      <c r="Y66" s="3"/>
-      <c r="Z66" s="3"/>
-      <c r="AA66" s="3"/>
-      <c r="AB66" s="3"/>
-      <c r="AC66" s="3"/>
-      <c r="AD66" s="3"/>
-      <c r="AE66" s="3"/>
-      <c r="AF66" s="3"/>
-      <c r="AG66" s="3"/>
-      <c r="AH66" s="3"/>
-      <c r="AI66" s="3"/>
-      <c r="AJ66" s="3"/>
-      <c r="AK66" s="3"/>
-      <c r="AL66" s="3"/>
-      <c r="AM66" s="3"/>
-      <c r="AN66" s="3"/>
-      <c r="AO66" s="3"/>
-      <c r="AP66" s="3"/>
-      <c r="AT66" s="3"/>
-    </row>
-    <row r="67" spans="15:54" x14ac:dyDescent="0.2">
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
-      <c r="R67" s="3"/>
-      <c r="S67" s="3"/>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
-      <c r="V67" s="3"/>
-      <c r="W67" s="3"/>
-      <c r="Y67" s="3"/>
-      <c r="Z67" s="3"/>
-      <c r="AA67" s="3"/>
-      <c r="AB67" s="3"/>
-      <c r="AC67" s="3"/>
-      <c r="AD67" s="3"/>
-      <c r="AE67" s="3"/>
-      <c r="AF67" s="3"/>
-      <c r="AG67" s="3"/>
-      <c r="AH67" s="3"/>
-      <c r="AI67" s="3"/>
-      <c r="AJ67" s="3"/>
-      <c r="AK67" s="3"/>
-      <c r="AL67" s="3"/>
-      <c r="AM67" s="3"/>
-      <c r="AN67" s="3"/>
-      <c r="AO67" s="3"/>
-      <c r="AP67" s="3"/>
-      <c r="AT67" s="3"/>
-    </row>
-    <row r="68" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="BR65" s="3"/>
+      <c r="BS65" s="3"/>
+      <c r="BT65" s="3"/>
+      <c r="BU65" s="3"/>
+      <c r="BV65" s="3"/>
+      <c r="BW65" s="3"/>
+      <c r="BX65" s="3"/>
+    </row>
+    <row r="66" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+      <c r="N66" s="10"/>
+      <c r="O66" s="10"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
+      <c r="U66" s="10"/>
+      <c r="V66" s="10"/>
+      <c r="W66" s="10"/>
+      <c r="X66" s="10"/>
+      <c r="Y66" s="10"/>
+      <c r="Z66" s="10"/>
+      <c r="AA66" s="10"/>
+      <c r="AB66" s="10"/>
+      <c r="AC66" s="10"/>
+      <c r="AD66" s="10"/>
+      <c r="AE66" s="10"/>
+      <c r="AF66" s="10"/>
+      <c r="AG66" s="10"/>
+      <c r="AH66" s="10"/>
+      <c r="AI66" s="10"/>
+      <c r="AJ66" s="10"/>
+      <c r="AK66" s="10"/>
+      <c r="AL66" s="10"/>
+      <c r="AM66" s="10"/>
+      <c r="AN66" s="10"/>
+      <c r="AO66" s="10"/>
+      <c r="AP66" s="10"/>
+      <c r="AQ66" s="10"/>
+      <c r="AR66" s="10"/>
+      <c r="AS66" s="10"/>
+      <c r="AT66" s="10"/>
+      <c r="AU66" s="10"/>
+      <c r="AV66" s="10"/>
+      <c r="AW66" s="10"/>
+      <c r="AX66" s="10"/>
+      <c r="AY66" s="10"/>
+      <c r="AZ66" s="10"/>
+      <c r="BA66" s="10"/>
+      <c r="BB66" s="10"/>
+      <c r="BC66" s="10"/>
+      <c r="BD66" s="3"/>
+      <c r="BE66" s="3"/>
+      <c r="BF66" s="3"/>
+      <c r="BG66" s="3"/>
+      <c r="BH66" s="3"/>
+      <c r="BI66" s="3"/>
+      <c r="BJ66" s="3"/>
+      <c r="BK66" s="3"/>
+      <c r="BL66" s="3"/>
+      <c r="BM66" s="3"/>
+      <c r="BN66" s="3"/>
+      <c r="BO66" s="3"/>
+      <c r="BP66" s="3"/>
+      <c r="BQ66" s="3"/>
+      <c r="BU66" s="10"/>
+    </row>
+    <row r="67" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10"/>
+      <c r="U67" s="10"/>
+      <c r="V67" s="10"/>
+      <c r="W67" s="10"/>
+      <c r="X67" s="10"/>
+      <c r="Y67" s="10"/>
+      <c r="Z67" s="10"/>
+      <c r="AA67" s="10"/>
+      <c r="AB67" s="10"/>
+      <c r="AC67" s="10"/>
+      <c r="AD67" s="10"/>
+      <c r="AE67" s="10"/>
+      <c r="AF67" s="10"/>
+      <c r="AG67" s="10"/>
+      <c r="AH67" s="10"/>
+      <c r="AI67" s="10"/>
+      <c r="AJ67" s="10"/>
+      <c r="AK67" s="10"/>
+      <c r="AL67" s="10"/>
+      <c r="AM67" s="10"/>
+      <c r="AN67" s="10"/>
+      <c r="AO67" s="10"/>
+      <c r="AP67" s="10"/>
+      <c r="AQ67" s="10"/>
+      <c r="AR67" s="10"/>
+      <c r="AS67" s="10"/>
+      <c r="AT67" s="10"/>
+      <c r="AU67" s="10"/>
+      <c r="AV67" s="10"/>
+      <c r="AW67" s="10"/>
+      <c r="AX67" s="10"/>
+      <c r="AY67" s="10"/>
+      <c r="AZ67" s="10"/>
+      <c r="BA67" s="10"/>
+      <c r="BB67" s="10"/>
+      <c r="BC67" s="10"/>
+      <c r="BD67" s="3"/>
+      <c r="BE67" s="3"/>
+      <c r="BF67" s="3"/>
+      <c r="BG67" s="3"/>
+      <c r="BH67" s="3"/>
+      <c r="BI67" s="3"/>
+      <c r="BJ67" s="3"/>
+      <c r="BK67" s="3"/>
+      <c r="BL67" s="3"/>
+      <c r="BM67" s="3"/>
+      <c r="BN67" s="3"/>
+      <c r="BO67" s="3"/>
+      <c r="BP67" s="3"/>
+      <c r="BQ67" s="3"/>
+      <c r="BU67" s="10"/>
+      <c r="BV67" s="3"/>
+      <c r="BW67" s="3"/>
+      <c r="BX67" s="3"/>
+      <c r="BY67" s="3"/>
+      <c r="BZ67" s="3"/>
+    </row>
+    <row r="68" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
       <c r="R68" s="3"/>
       <c r="S68" s="3"/>
-      <c r="T68" s="3"/>
-      <c r="U68" s="3"/>
-      <c r="V68" s="3"/>
-      <c r="W68" s="3"/>
-      <c r="Y68" s="3"/>
-      <c r="Z68" s="3"/>
-      <c r="AA68" s="3"/>
-      <c r="AB68" s="3"/>
-      <c r="AC68" s="3"/>
-      <c r="AD68" s="3"/>
-      <c r="AE68" s="3"/>
-      <c r="AF68" s="3"/>
-      <c r="AG68" s="3"/>
-      <c r="AH68" s="3"/>
-      <c r="AI68" s="3"/>
-      <c r="AJ68" s="3"/>
-      <c r="AK68" s="3"/>
-      <c r="AL68" s="3"/>
-      <c r="AM68" s="3"/>
       <c r="AN68" s="3"/>
       <c r="AO68" s="3"/>
       <c r="AP68" s="3"/>
       <c r="AT68" s="3"/>
-    </row>
-    <row r="69" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="AX68" s="3"/>
+      <c r="AY68" s="3"/>
+      <c r="AZ68" s="3"/>
+      <c r="BA68" s="3"/>
+      <c r="BC68" s="10"/>
+      <c r="BD68" s="3"/>
+      <c r="BE68" s="3"/>
+      <c r="BF68" s="3"/>
+      <c r="BG68" s="3"/>
+      <c r="BH68" s="3"/>
+      <c r="BI68" s="3"/>
+      <c r="BJ68" s="3"/>
+      <c r="BK68" s="3"/>
+      <c r="BL68" s="3"/>
+      <c r="BM68" s="3"/>
+      <c r="BN68" s="3"/>
+      <c r="BO68" s="3"/>
+      <c r="BP68" s="3"/>
+      <c r="BQ68" s="3"/>
+      <c r="BU68" s="10"/>
+      <c r="BV68" s="3"/>
+      <c r="BW68" s="3"/>
+      <c r="BX68" s="3"/>
+      <c r="BY68" s="3"/>
+      <c r="BZ68" s="3"/>
+    </row>
+    <row r="69" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
       <c r="R69" s="3"/>
       <c r="S69" s="3"/>
-      <c r="T69" s="3"/>
-      <c r="U69" s="3"/>
-      <c r="V69" s="3"/>
-      <c r="W69" s="3"/>
-      <c r="Y69" s="3"/>
-      <c r="Z69" s="3"/>
-      <c r="AA69" s="3"/>
-      <c r="AB69" s="3"/>
-      <c r="AC69" s="3"/>
-      <c r="AD69" s="3"/>
-      <c r="AE69" s="3"/>
-      <c r="AF69" s="3"/>
-      <c r="AG69" s="3"/>
-      <c r="AH69" s="3"/>
-      <c r="AI69" s="3"/>
-      <c r="AJ69" s="3"/>
-      <c r="AK69" s="3"/>
-      <c r="AL69" s="3"/>
-      <c r="AM69" s="3"/>
       <c r="AN69" s="3"/>
       <c r="AO69" s="3"/>
       <c r="AP69" s="3"/>
       <c r="AT69" s="3"/>
-    </row>
-    <row r="70" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="AX69" s="3"/>
+      <c r="AY69" s="3"/>
+      <c r="AZ69" s="3"/>
+      <c r="BA69" s="3"/>
+      <c r="BC69" s="10"/>
+      <c r="BD69" s="3"/>
+      <c r="BE69" s="3"/>
+      <c r="BF69" s="3"/>
+      <c r="BG69" s="3"/>
+      <c r="BH69" s="3"/>
+      <c r="BI69" s="3"/>
+      <c r="BJ69" s="3"/>
+      <c r="BK69" s="3"/>
+      <c r="BL69" s="3"/>
+      <c r="BM69" s="3"/>
+      <c r="BN69" s="3"/>
+      <c r="BO69" s="3"/>
+      <c r="BP69" s="3"/>
+      <c r="BQ69" s="3"/>
+      <c r="BU69" s="10"/>
+      <c r="BV69" s="3"/>
+      <c r="BW69" s="3"/>
+      <c r="BX69" s="3"/>
+      <c r="BY69" s="3"/>
+      <c r="BZ69" s="3"/>
+    </row>
+    <row r="70" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
       <c r="S70" s="3"/>
-      <c r="T70" s="3"/>
-      <c r="U70" s="3"/>
-      <c r="V70" s="3"/>
-      <c r="W70" s="3"/>
-      <c r="Y70" s="3"/>
-      <c r="Z70" s="3"/>
-      <c r="AA70" s="3"/>
-      <c r="AB70" s="3"/>
-      <c r="AC70" s="3"/>
-      <c r="AD70" s="3"/>
-      <c r="AE70" s="3"/>
-      <c r="AF70" s="3"/>
-      <c r="AG70" s="3"/>
-      <c r="AH70" s="3"/>
-      <c r="AI70" s="3"/>
-      <c r="AJ70" s="3"/>
-      <c r="AK70" s="3"/>
-      <c r="AL70" s="3"/>
-      <c r="AM70" s="3"/>
       <c r="AN70" s="3"/>
       <c r="AO70" s="3"/>
       <c r="AP70" s="3"/>
       <c r="AQ70" s="3"/>
       <c r="AT70" s="3"/>
-    </row>
-    <row r="71" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="AX70" s="3"/>
+      <c r="AY70" s="3"/>
+      <c r="AZ70" s="3"/>
+      <c r="BA70" s="3"/>
+      <c r="BC70" s="17"/>
+      <c r="BD70" s="17"/>
+      <c r="BE70" s="3"/>
+      <c r="BF70" s="3"/>
+      <c r="BG70" s="3"/>
+      <c r="BH70" s="3"/>
+      <c r="BI70" s="3"/>
+      <c r="BJ70" s="3"/>
+      <c r="BK70" s="3"/>
+      <c r="BL70" s="3"/>
+      <c r="BM70" s="3"/>
+      <c r="BN70" s="3"/>
+      <c r="BO70" s="3"/>
+      <c r="BP70" s="3"/>
+      <c r="BQ70" s="3"/>
+      <c r="BU70" s="10"/>
+      <c r="BV70" s="3"/>
+      <c r="BW70" s="3"/>
+      <c r="BX70" s="3"/>
+      <c r="BY70" s="3"/>
+      <c r="BZ70" s="3"/>
+    </row>
+    <row r="71" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
       <c r="R71" s="3"/>
       <c r="S71" s="15"/>
-      <c r="T71" s="3"/>
-      <c r="U71" s="3"/>
-      <c r="V71" s="3"/>
-      <c r="W71" s="3"/>
-      <c r="Y71" s="3"/>
-      <c r="Z71" s="3"/>
-      <c r="AA71" s="3"/>
-      <c r="AB71" s="3"/>
-      <c r="AC71" s="3"/>
-      <c r="AD71" s="3"/>
-      <c r="AE71" s="3"/>
-      <c r="AF71" s="3"/>
-      <c r="AG71" s="3"/>
-      <c r="AH71" s="3"/>
-      <c r="AI71" s="3"/>
-      <c r="AJ71" s="3"/>
-      <c r="AK71" s="3"/>
-      <c r="AL71" s="3"/>
-      <c r="AM71" s="3"/>
       <c r="AN71" s="3"/>
       <c r="AO71" s="3"/>
       <c r="AP71" s="3"/>
       <c r="AQ71" s="3"/>
       <c r="AT71" s="3"/>
-    </row>
-    <row r="72" spans="15:54" x14ac:dyDescent="0.2">
-      <c r="O72" s="3"/>
-      <c r="P72" s="3"/>
-      <c r="Q72" s="3"/>
-      <c r="R72" s="3"/>
-      <c r="S72" s="3"/>
-      <c r="T72" s="3"/>
-      <c r="U72" s="3"/>
-      <c r="V72" s="3"/>
-      <c r="W72" s="3"/>
-      <c r="X72" s="3"/>
-      <c r="Y72" s="3"/>
-      <c r="Z72" s="3"/>
-      <c r="AA72" s="3"/>
-      <c r="AB72" s="3"/>
-      <c r="AC72" s="3"/>
-      <c r="AD72" s="3"/>
-      <c r="AE72" s="3"/>
-      <c r="AF72" s="5"/>
-      <c r="AG72" s="5"/>
-      <c r="AH72" s="5"/>
-      <c r="AI72" s="15"/>
-      <c r="AJ72" s="3"/>
-      <c r="AK72" s="3"/>
-      <c r="AL72" s="3"/>
-      <c r="AM72" s="3"/>
-      <c r="AN72" s="3"/>
-      <c r="AO72" s="3"/>
-      <c r="AP72" s="3"/>
-      <c r="AT72" s="3"/>
-    </row>
-    <row r="73" spans="15:54" x14ac:dyDescent="0.2">
-      <c r="O73" s="3"/>
-      <c r="P73" s="3"/>
-      <c r="Q73" s="3"/>
-      <c r="R73" s="3"/>
-      <c r="S73" s="3"/>
-      <c r="T73" s="3"/>
-      <c r="U73" s="3"/>
-      <c r="V73" s="3"/>
-      <c r="W73" s="3"/>
-      <c r="Y73" s="3"/>
-      <c r="Z73" s="3"/>
-      <c r="AA73" s="3"/>
-      <c r="AB73" s="3"/>
-      <c r="AC73" s="3"/>
-      <c r="AD73" s="3"/>
-      <c r="AE73" s="3"/>
-      <c r="AF73" s="3"/>
-      <c r="AG73" s="3"/>
-      <c r="AH73" s="3"/>
-      <c r="AI73" s="3"/>
-      <c r="AJ73" s="3"/>
-      <c r="AK73" s="3"/>
-      <c r="AL73" s="3"/>
-      <c r="AM73" s="3"/>
-      <c r="AN73" s="3"/>
-      <c r="AO73" s="3"/>
-      <c r="AP73" s="3"/>
-      <c r="AT73" s="3"/>
-    </row>
-    <row r="74" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="AX71" s="3"/>
+      <c r="AY71" s="3"/>
+      <c r="AZ71" s="3"/>
+      <c r="BA71" s="3"/>
+      <c r="BC71" s="17"/>
+      <c r="BD71" s="17"/>
+      <c r="BE71" s="3"/>
+      <c r="BF71" s="3"/>
+      <c r="BG71" s="3"/>
+      <c r="BH71" s="3"/>
+      <c r="BI71" s="3"/>
+      <c r="BJ71" s="3"/>
+      <c r="BK71" s="3"/>
+      <c r="BL71" s="3"/>
+      <c r="BM71" s="3"/>
+      <c r="BN71" s="3"/>
+      <c r="BO71" s="3"/>
+      <c r="BP71" s="3"/>
+      <c r="BQ71" s="3"/>
+      <c r="BU71" s="10"/>
+      <c r="BV71" s="3"/>
+      <c r="BW71" s="3"/>
+      <c r="BX71" s="3"/>
+      <c r="BY71" s="3"/>
+      <c r="BZ71" s="3"/>
+    </row>
+    <row r="72" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
+      <c r="O72" s="10"/>
+      <c r="P72" s="10"/>
+      <c r="Q72" s="10"/>
+      <c r="R72" s="10"/>
+      <c r="S72" s="10"/>
+      <c r="T72" s="10"/>
+      <c r="U72" s="10"/>
+      <c r="V72" s="10"/>
+      <c r="W72" s="10"/>
+      <c r="X72" s="10"/>
+      <c r="Y72" s="10"/>
+      <c r="Z72" s="10"/>
+      <c r="AA72" s="10"/>
+      <c r="AB72" s="10"/>
+      <c r="AC72" s="10"/>
+      <c r="AD72" s="10"/>
+      <c r="AE72" s="10"/>
+      <c r="AF72" s="10"/>
+      <c r="AG72" s="10"/>
+      <c r="AH72" s="10"/>
+      <c r="AI72" s="10"/>
+      <c r="AJ72" s="10"/>
+      <c r="AK72" s="10"/>
+      <c r="AL72" s="10"/>
+      <c r="AM72" s="10"/>
+      <c r="AN72" s="10"/>
+      <c r="AO72" s="10"/>
+      <c r="AP72" s="10"/>
+      <c r="AQ72" s="10"/>
+      <c r="AR72" s="10"/>
+      <c r="AS72" s="10"/>
+      <c r="AT72" s="10"/>
+      <c r="AU72" s="10"/>
+      <c r="AV72" s="10"/>
+      <c r="AW72" s="10"/>
+      <c r="AX72" s="10"/>
+      <c r="AY72" s="10"/>
+      <c r="AZ72" s="10"/>
+      <c r="BA72" s="3"/>
+      <c r="BB72" s="10"/>
+      <c r="BC72" s="10"/>
+      <c r="BD72" s="10"/>
+      <c r="BE72" s="10"/>
+      <c r="BF72" s="10"/>
+      <c r="BG72" s="10"/>
+      <c r="BH72" s="10"/>
+      <c r="BI72" s="10"/>
+      <c r="BJ72" s="18"/>
+      <c r="BK72" s="18"/>
+      <c r="BL72" s="18"/>
+      <c r="BM72" s="19"/>
+      <c r="BN72" s="10"/>
+      <c r="BO72" s="10"/>
+      <c r="BP72" s="10"/>
+      <c r="BQ72" s="3"/>
+      <c r="BS72" s="10"/>
+      <c r="BU72" s="10"/>
+      <c r="BV72" s="3"/>
+      <c r="BW72" s="3"/>
+      <c r="BX72" s="3"/>
+      <c r="BY72" s="3"/>
+      <c r="BZ72" s="3"/>
+    </row>
+    <row r="73" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
+      <c r="M73" s="10"/>
+      <c r="N73" s="10"/>
+      <c r="O73" s="10"/>
+      <c r="P73" s="10"/>
+      <c r="Q73" s="10"/>
+      <c r="R73" s="10"/>
+      <c r="S73" s="10"/>
+      <c r="T73" s="10"/>
+      <c r="U73" s="10"/>
+      <c r="V73" s="10"/>
+      <c r="W73" s="10"/>
+      <c r="X73" s="10"/>
+      <c r="Y73" s="10"/>
+      <c r="Z73" s="10"/>
+      <c r="AA73" s="10"/>
+      <c r="AB73" s="10"/>
+      <c r="AC73" s="10"/>
+      <c r="AD73" s="10"/>
+      <c r="AE73" s="10"/>
+      <c r="AF73" s="10"/>
+      <c r="AG73" s="10"/>
+      <c r="AH73" s="10"/>
+      <c r="AI73" s="10"/>
+      <c r="AJ73" s="10"/>
+      <c r="AK73" s="10"/>
+      <c r="AL73" s="10"/>
+      <c r="AM73" s="10"/>
+      <c r="AN73" s="10"/>
+      <c r="AO73" s="10"/>
+      <c r="AP73" s="10"/>
+      <c r="AQ73" s="10"/>
+      <c r="AR73" s="10"/>
+      <c r="AS73" s="10"/>
+      <c r="AT73" s="10"/>
+      <c r="AU73" s="10"/>
+      <c r="AV73" s="10"/>
+      <c r="AW73" s="10"/>
+      <c r="AX73" s="10"/>
+      <c r="AY73" s="10"/>
+      <c r="AZ73" s="10"/>
+      <c r="BA73" s="3"/>
+      <c r="BB73" s="3"/>
+      <c r="BC73" s="3"/>
+      <c r="BD73" s="3"/>
+      <c r="BE73" s="3"/>
+      <c r="BF73" s="3"/>
+      <c r="BG73" s="3"/>
+      <c r="BH73" s="3"/>
+      <c r="BI73" s="3"/>
+      <c r="BJ73" s="3"/>
+      <c r="BK73" s="3"/>
+      <c r="BL73" s="3"/>
+      <c r="BM73" s="3"/>
+      <c r="BN73" s="3"/>
+      <c r="BO73" s="3"/>
+      <c r="BP73" s="3"/>
+      <c r="BQ73" s="3"/>
+      <c r="BR73" s="10"/>
+      <c r="BS73" s="10"/>
+      <c r="BU73" s="10"/>
+    </row>
+    <row r="74" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
       <c r="Q74" s="3"/>
       <c r="R74" s="3"/>
       <c r="S74" s="3"/>
-      <c r="T74" s="3"/>
-      <c r="U74" s="3"/>
-      <c r="V74" s="3"/>
-      <c r="W74" s="3"/>
-      <c r="Y74" s="3"/>
-      <c r="Z74" s="3"/>
-      <c r="AA74" s="3"/>
-      <c r="AB74" s="3"/>
-      <c r="AC74" s="3"/>
-      <c r="AD74" s="3"/>
-      <c r="AE74" s="3"/>
-      <c r="AF74" s="3"/>
-      <c r="AG74" s="3"/>
-      <c r="AH74" s="3"/>
-      <c r="AI74" s="3"/>
-      <c r="AJ74" s="3"/>
-      <c r="AK74" s="3"/>
-      <c r="AL74" s="3"/>
-      <c r="AM74" s="3"/>
       <c r="AN74" s="3"/>
       <c r="AO74" s="3"/>
       <c r="AP74" s="3"/>
       <c r="AT74" s="3"/>
-    </row>
-    <row r="75" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="AX74" s="3"/>
+      <c r="AY74" s="10"/>
+      <c r="AZ74" s="10"/>
+      <c r="BA74" s="3"/>
+      <c r="BB74" s="3"/>
+      <c r="BC74" s="3"/>
+      <c r="BD74" s="3"/>
+      <c r="BE74" s="3"/>
+      <c r="BF74" s="3"/>
+      <c r="BG74" s="3"/>
+      <c r="BH74" s="3"/>
+      <c r="BI74" s="3"/>
+      <c r="BJ74" s="3"/>
+      <c r="BK74" s="3"/>
+      <c r="BL74" s="3"/>
+      <c r="BM74" s="3"/>
+      <c r="BN74" s="3"/>
+      <c r="BO74" s="3"/>
+      <c r="BP74" s="3"/>
+      <c r="BQ74" s="10"/>
+      <c r="BR74" s="10"/>
+      <c r="BS74" s="10"/>
+      <c r="BU74" s="10"/>
+    </row>
+    <row r="75" spans="6:78" x14ac:dyDescent="0.2">
       <c r="O75" s="3"/>
       <c r="P75" s="3"/>
       <c r="Q75" s="3"/>
       <c r="R75" s="3"/>
       <c r="S75" s="3"/>
-      <c r="T75" s="3"/>
-      <c r="U75" s="3"/>
-      <c r="V75" s="3"/>
-      <c r="W75" s="3"/>
-      <c r="X75" s="3"/>
-      <c r="Y75" s="3"/>
-      <c r="Z75" s="3"/>
-      <c r="AA75" s="3"/>
-      <c r="AB75" s="3"/>
-      <c r="AC75" s="3"/>
-      <c r="AD75" s="3"/>
-      <c r="AE75" s="3"/>
-      <c r="AF75" s="3"/>
-      <c r="AG75" s="3"/>
-      <c r="AH75" s="3"/>
-      <c r="AI75" s="3"/>
-      <c r="AJ75" s="3"/>
-      <c r="AK75" s="3"/>
-      <c r="AL75" s="3"/>
-      <c r="AM75" s="3"/>
       <c r="AN75" s="3"/>
       <c r="AO75" s="3"/>
       <c r="AP75" s="3"/>
@@ -1622,30 +1931,33 @@
       <c r="AS75" s="3"/>
       <c r="AT75" s="3"/>
       <c r="AU75" s="3"/>
-    </row>
-    <row r="76" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="AX75" s="3"/>
+      <c r="AY75" s="10"/>
+      <c r="AZ75" s="10"/>
+      <c r="BA75" s="10"/>
+      <c r="BB75" s="10"/>
+      <c r="BC75" s="10"/>
+      <c r="BD75" s="10"/>
+      <c r="BE75" s="10"/>
+      <c r="BF75" s="10"/>
+      <c r="BG75" s="10"/>
+      <c r="BH75" s="10"/>
+      <c r="BI75" s="10"/>
+      <c r="BJ75" s="10"/>
+      <c r="BK75" s="10"/>
+      <c r="BL75" s="10"/>
+      <c r="BM75" s="10"/>
+      <c r="BN75" s="10"/>
+      <c r="BO75" s="10"/>
+      <c r="BP75" s="10"/>
+      <c r="BQ75" s="10"/>
+      <c r="BR75" s="10"/>
+      <c r="BS75" s="10"/>
+      <c r="BU75" s="10"/>
+    </row>
+    <row r="76" spans="6:78" x14ac:dyDescent="0.2">
       <c r="R76" s="3"/>
       <c r="S76" s="3"/>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
-      <c r="W76" s="3"/>
-      <c r="X76" s="3"/>
-      <c r="Y76" s="3"/>
-      <c r="Z76" s="3"/>
-      <c r="AA76" s="3"/>
-      <c r="AB76" s="3"/>
-      <c r="AC76" s="3"/>
-      <c r="AD76" s="3"/>
-      <c r="AE76" s="3"/>
-      <c r="AF76" s="3"/>
-      <c r="AG76" s="3"/>
-      <c r="AH76" s="3"/>
-      <c r="AI76" s="3"/>
-      <c r="AJ76" s="3"/>
-      <c r="AK76" s="3"/>
-      <c r="AL76" s="3"/>
-      <c r="AM76" s="3"/>
       <c r="AN76" s="3"/>
       <c r="AO76" s="3"/>
       <c r="AP76" s="3"/>
@@ -1654,32 +1966,31 @@
       <c r="AS76" s="3"/>
       <c r="AT76" s="3"/>
       <c r="AU76" s="3"/>
+      <c r="AX76" s="3"/>
+      <c r="AY76" s="10"/>
+      <c r="AZ76" s="3"/>
       <c r="BA76" s="3"/>
       <c r="BB76" s="3"/>
-    </row>
-    <row r="77" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="BC76" s="3"/>
+      <c r="BD76" s="3"/>
+      <c r="BE76" s="3"/>
+      <c r="BF76" s="3"/>
+      <c r="BG76" s="3"/>
+      <c r="BH76" s="3"/>
+      <c r="BI76" s="3"/>
+      <c r="BJ76" s="3"/>
+      <c r="BK76" s="3"/>
+      <c r="BL76" s="3"/>
+      <c r="BM76" s="3"/>
+      <c r="BN76" s="3"/>
+      <c r="BO76" s="3"/>
+      <c r="BP76" s="3"/>
+      <c r="BQ76" s="3"/>
+      <c r="BU76" s="10"/>
+    </row>
+    <row r="77" spans="6:78" x14ac:dyDescent="0.2">
       <c r="R77" s="3"/>
       <c r="S77" s="3"/>
-      <c r="T77" s="3"/>
-      <c r="U77" s="3"/>
-      <c r="V77" s="3"/>
-      <c r="W77" s="3"/>
-      <c r="X77" s="3"/>
-      <c r="Y77" s="3"/>
-      <c r="Z77" s="3"/>
-      <c r="AA77" s="3"/>
-      <c r="AB77" s="3"/>
-      <c r="AC77" s="3"/>
-      <c r="AD77" s="3"/>
-      <c r="AE77" s="3"/>
-      <c r="AF77" s="3"/>
-      <c r="AG77" s="3"/>
-      <c r="AH77" s="3"/>
-      <c r="AI77" s="3"/>
-      <c r="AJ77" s="3"/>
-      <c r="AK77" s="3"/>
-      <c r="AL77" s="3"/>
-      <c r="AM77" s="3"/>
       <c r="AN77" s="3"/>
       <c r="AO77" s="3"/>
       <c r="AP77" s="3"/>
@@ -1691,34 +2002,36 @@
       <c r="AV77" s="3"/>
       <c r="AW77" s="3"/>
       <c r="AX77" s="3"/>
-      <c r="AY77" s="3"/>
+      <c r="AY77" s="10"/>
       <c r="AZ77" s="3"/>
       <c r="BA77" s="3"/>
       <c r="BB77" s="3"/>
-    </row>
-    <row r="78" spans="15:54" x14ac:dyDescent="0.2">
-      <c r="R78" s="3"/>
-      <c r="S78" s="3"/>
-      <c r="T78" s="3"/>
-      <c r="U78" s="3"/>
-      <c r="V78" s="3"/>
-      <c r="W78" s="3"/>
-      <c r="X78" s="3"/>
-      <c r="Y78" s="3"/>
-      <c r="Z78" s="3"/>
-      <c r="AA78" s="3"/>
-      <c r="AB78" s="3"/>
-      <c r="AC78" s="3"/>
-      <c r="AD78" s="3"/>
-      <c r="AE78" s="3"/>
-      <c r="AF78" s="3"/>
-      <c r="AG78" s="3"/>
-      <c r="AH78" s="3"/>
-      <c r="AI78" s="3"/>
-      <c r="AJ78" s="3"/>
-      <c r="AK78" s="3"/>
-      <c r="AL78" s="3"/>
-      <c r="AM78" s="3"/>
+      <c r="BC77" s="3"/>
+      <c r="BD77" s="3"/>
+      <c r="BE77" s="3"/>
+      <c r="BF77" s="3"/>
+      <c r="BG77" s="3"/>
+      <c r="BH77" s="3"/>
+      <c r="BI77" s="3"/>
+      <c r="BJ77" s="3"/>
+      <c r="BK77" s="3"/>
+      <c r="BL77" s="3"/>
+      <c r="BM77" s="3"/>
+      <c r="BN77" s="3"/>
+      <c r="BO77" s="3"/>
+      <c r="BP77" s="3"/>
+      <c r="BQ77" s="3"/>
+      <c r="BU77" s="10"/>
+    </row>
+    <row r="78" spans="6:78" x14ac:dyDescent="0.2">
+      <c r="M78" s="16"/>
+      <c r="N78" s="16"/>
+      <c r="O78" s="16"/>
+      <c r="P78" s="16"/>
+      <c r="Q78" s="16"/>
+      <c r="R78" s="16"/>
+      <c r="S78" s="16"/>
+      <c r="T78" s="16"/>
       <c r="AN78" s="3"/>
       <c r="AO78" s="3"/>
       <c r="AP78" s="3"/>
@@ -1730,12 +2043,28 @@
       <c r="AV78" s="3"/>
       <c r="AW78" s="3"/>
       <c r="AX78" s="3"/>
-      <c r="AY78" s="3"/>
+      <c r="AY78" s="10"/>
       <c r="AZ78" s="3"/>
       <c r="BA78" s="3"/>
       <c r="BB78" s="3"/>
-    </row>
-    <row r="79" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="BC78" s="3"/>
+      <c r="BD78" s="3"/>
+      <c r="BE78" s="3"/>
+      <c r="BF78" s="3"/>
+      <c r="BG78" s="3"/>
+      <c r="BH78" s="3"/>
+      <c r="BI78" s="3"/>
+      <c r="BJ78" s="3"/>
+      <c r="BK78" s="3"/>
+      <c r="BL78" s="3"/>
+      <c r="BM78" s="3"/>
+      <c r="BN78" s="3"/>
+      <c r="BO78" s="3"/>
+      <c r="BP78" s="3"/>
+      <c r="BQ78" s="3"/>
+      <c r="BU78" s="10"/>
+    </row>
+    <row r="79" spans="6:78" x14ac:dyDescent="0.2">
       <c r="R79" s="3"/>
       <c r="AO79" s="3"/>
       <c r="AP79" s="3"/>
@@ -1743,10 +2072,30 @@
       <c r="AR79" s="3"/>
       <c r="AS79" s="14"/>
       <c r="AT79" s="14"/>
-      <c r="BA79" s="3"/>
-      <c r="BB79" s="3"/>
-    </row>
-    <row r="80" spans="15:54" x14ac:dyDescent="0.2">
+      <c r="AY79" s="10"/>
+      <c r="BA79" s="10"/>
+      <c r="BB79" s="10"/>
+      <c r="BC79" s="10"/>
+      <c r="BD79" s="10"/>
+      <c r="BE79" s="10"/>
+      <c r="BF79" s="10"/>
+      <c r="BG79" s="10"/>
+      <c r="BH79" s="10"/>
+      <c r="BI79" s="10"/>
+      <c r="BJ79" s="10"/>
+      <c r="BK79" s="10"/>
+      <c r="BL79" s="10"/>
+      <c r="BM79" s="10"/>
+      <c r="BN79" s="10"/>
+      <c r="BO79" s="10"/>
+      <c r="BP79" s="10"/>
+      <c r="BQ79" s="10"/>
+      <c r="BR79" s="10"/>
+      <c r="BS79" s="10"/>
+      <c r="BT79" s="10"/>
+      <c r="BU79" s="10"/>
+    </row>
+    <row r="80" spans="6:78" x14ac:dyDescent="0.2">
       <c r="R80" s="3"/>
       <c r="AO80" s="3"/>
       <c r="AP80" s="3"/>
@@ -1756,10 +2105,30 @@
       <c r="AU80" s="3"/>
       <c r="AV80" s="3"/>
       <c r="AW80" s="3"/>
-      <c r="BA80" s="3"/>
-      <c r="BB80" s="3"/>
-    </row>
-    <row r="81" spans="8:54" x14ac:dyDescent="0.2">
+      <c r="AY80" s="10"/>
+      <c r="BA80" s="10"/>
+      <c r="BB80" s="10"/>
+      <c r="BC80" s="10"/>
+      <c r="BD80" s="10"/>
+      <c r="BE80" s="10"/>
+      <c r="BF80" s="10"/>
+      <c r="BG80" s="10"/>
+      <c r="BH80" s="10"/>
+      <c r="BI80" s="10"/>
+      <c r="BJ80" s="10"/>
+      <c r="BK80" s="10"/>
+      <c r="BL80" s="10"/>
+      <c r="BM80" s="10"/>
+      <c r="BN80" s="10"/>
+      <c r="BO80" s="10"/>
+      <c r="BP80" s="10"/>
+      <c r="BQ80" s="10"/>
+      <c r="BR80" s="10"/>
+      <c r="BS80" s="10"/>
+      <c r="BT80" s="10"/>
+      <c r="BU80" s="10"/>
+    </row>
+    <row r="81" spans="5:74" x14ac:dyDescent="0.2">
       <c r="R81" s="3"/>
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
@@ -1790,11 +2159,12 @@
       <c r="AS81" s="3"/>
       <c r="AT81" s="3"/>
       <c r="AU81" s="3"/>
-      <c r="AY81" s="3"/>
+      <c r="AY81" s="10"/>
       <c r="BA81" s="3"/>
       <c r="BB81" s="3"/>
-    </row>
-    <row r="82" spans="8:54" x14ac:dyDescent="0.2">
+      <c r="BV81" s="10"/>
+    </row>
+    <row r="82" spans="5:74" x14ac:dyDescent="0.2">
       <c r="R82" s="3"/>
       <c r="T82" s="3"/>
       <c r="U82" s="3"/>
@@ -1827,11 +2197,12 @@
       <c r="AV82" s="3"/>
       <c r="AW82" s="3"/>
       <c r="AX82" s="3"/>
-      <c r="AY82" s="3"/>
+      <c r="AY82" s="10"/>
       <c r="BA82" s="3"/>
       <c r="BB82" s="3"/>
-    </row>
-    <row r="83" spans="8:54" x14ac:dyDescent="0.2">
+      <c r="BV82" s="10"/>
+    </row>
+    <row r="83" spans="5:74" x14ac:dyDescent="0.2">
       <c r="R83" s="3"/>
       <c r="Z83" s="3"/>
       <c r="AA83" s="3"/>
@@ -1852,11 +2223,12 @@
       <c r="AV83" s="3"/>
       <c r="AW83" s="3"/>
       <c r="AX83" s="3"/>
-      <c r="AY83" s="3"/>
+      <c r="AY83" s="10"/>
       <c r="BA83" s="3"/>
       <c r="BB83" s="3"/>
-    </row>
-    <row r="84" spans="8:54" x14ac:dyDescent="0.2">
+      <c r="BV83" s="10"/>
+    </row>
+    <row r="84" spans="5:74" x14ac:dyDescent="0.2">
       <c r="R84" s="3"/>
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
@@ -1890,11 +2262,12 @@
       <c r="AV84" s="3"/>
       <c r="AW84" s="3"/>
       <c r="AX84" s="3"/>
-      <c r="AY84" s="3"/>
+      <c r="AY84" s="10"/>
       <c r="BA84" s="3"/>
       <c r="BB84" s="3"/>
-    </row>
-    <row r="85" spans="8:54" x14ac:dyDescent="0.2">
+      <c r="BV84" s="10"/>
+    </row>
+    <row r="85" spans="5:74" x14ac:dyDescent="0.2">
       <c r="X85" s="3"/>
       <c r="Y85" s="3"/>
       <c r="Z85" s="3"/>
@@ -1922,11 +2295,32 @@
       <c r="AV85" s="3"/>
       <c r="AW85" s="3"/>
       <c r="AX85" s="3"/>
-      <c r="AY85" s="3"/>
-      <c r="BA85" s="3"/>
-      <c r="BB85" s="3"/>
-    </row>
-    <row r="86" spans="8:54" x14ac:dyDescent="0.2">
+      <c r="AY85" s="10"/>
+      <c r="AZ85" s="10"/>
+      <c r="BA85" s="10"/>
+      <c r="BB85" s="10"/>
+      <c r="BC85" s="10"/>
+      <c r="BD85" s="10"/>
+      <c r="BE85" s="10"/>
+      <c r="BF85" s="10"/>
+      <c r="BG85" s="10"/>
+      <c r="BH85" s="10"/>
+      <c r="BI85" s="10"/>
+      <c r="BJ85" s="10"/>
+      <c r="BK85" s="10"/>
+      <c r="BL85" s="10"/>
+      <c r="BM85" s="10"/>
+      <c r="BN85" s="10"/>
+      <c r="BO85" s="10"/>
+      <c r="BP85" s="10"/>
+      <c r="BQ85" s="10"/>
+      <c r="BR85" s="10"/>
+      <c r="BS85" s="10"/>
+      <c r="BT85" s="10"/>
+      <c r="BU85" s="10"/>
+      <c r="BV85" s="10"/>
+    </row>
+    <row r="86" spans="5:74" x14ac:dyDescent="0.2">
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
@@ -1963,10 +2357,11 @@
       <c r="BA86" s="3"/>
       <c r="BB86" s="3"/>
     </row>
-    <row r="87" spans="8:54" x14ac:dyDescent="0.2">
-      <c r="H87" s="13" t="s">
-        <v>6</v>
+    <row r="87" spans="5:74" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>1</v>
       </c>
+      <c r="H87" s="13"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
@@ -2005,7 +2400,7 @@
       <c r="BA87" s="3"/>
       <c r="BB87" s="3"/>
     </row>
-    <row r="88" spans="8:54" x14ac:dyDescent="0.2">
+    <row r="88" spans="5:74" x14ac:dyDescent="0.2">
       <c r="X88" s="3"/>
       <c r="Y88" s="3"/>
       <c r="Z88" s="3"/>
@@ -2038,7 +2433,7 @@
       <c r="BA88" s="3"/>
       <c r="BB88" s="3"/>
     </row>
-    <row r="89" spans="8:54" x14ac:dyDescent="0.2">
+    <row r="89" spans="5:74" x14ac:dyDescent="0.2">
       <c r="X89" s="3"/>
       <c r="Y89" s="3"/>
       <c r="Z89" s="3"/>
@@ -2071,7 +2466,7 @@
       <c r="BA89" s="3"/>
       <c r="BB89" s="3"/>
     </row>
-    <row r="90" spans="8:54" x14ac:dyDescent="0.2">
+    <row r="90" spans="5:74" x14ac:dyDescent="0.2">
       <c r="X90" s="3"/>
       <c r="Y90" s="3"/>
       <c r="Z90" s="3"/>
@@ -2104,7 +2499,7 @@
       <c r="BA90" s="3"/>
       <c r="BB90" s="3"/>
     </row>
-    <row r="91" spans="8:54" x14ac:dyDescent="0.2">
+    <row r="91" spans="5:74" x14ac:dyDescent="0.2">
       <c r="X91" s="3"/>
       <c r="Y91" s="3"/>
       <c r="Z91" s="3"/>
@@ -2121,7 +2516,7 @@
       <c r="AK91" s="3"/>
       <c r="AO91" s="3"/>
     </row>
-    <row r="92" spans="8:54" x14ac:dyDescent="0.2">
+    <row r="92" spans="5:74" x14ac:dyDescent="0.2">
       <c r="X92" s="3"/>
       <c r="Y92" s="3"/>
       <c r="Z92" s="3"/>
@@ -2138,10 +2533,7 @@
       <c r="AK92" s="3"/>
       <c r="AO92" s="3"/>
     </row>
-    <row r="93" spans="8:54" x14ac:dyDescent="0.2">
-      <c r="R93" t="s">
-        <v>1</v>
-      </c>
+    <row r="93" spans="5:74" x14ac:dyDescent="0.2">
       <c r="Z93" s="3"/>
       <c r="AA93" s="3"/>
       <c r="AB93" s="3"/>
@@ -2156,15 +2548,1130 @@
       <c r="AK93" s="3"/>
       <c r="AO93" s="3"/>
     </row>
+    <row r="99" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="Y99" s="3"/>
+      <c r="Z99" s="3"/>
+      <c r="AA99" s="3"/>
+      <c r="AB99" s="3"/>
+      <c r="AC99" s="3"/>
+      <c r="AD99" s="3"/>
+      <c r="AE99" s="3"/>
+      <c r="AF99" s="3"/>
+      <c r="AG99" s="3"/>
+      <c r="AH99" s="3"/>
+      <c r="AI99" s="3"/>
+      <c r="AJ99" s="3"/>
+      <c r="AK99" s="3"/>
+      <c r="AL99" s="3"/>
+      <c r="AM99" s="3"/>
+      <c r="AN99" s="3"/>
+      <c r="AO99" s="3"/>
+      <c r="AP99" s="3"/>
+      <c r="AQ99" s="3"/>
+      <c r="AR99" s="3"/>
+      <c r="AS99" s="3"/>
+      <c r="AT99" s="3"/>
+      <c r="AU99" s="3"/>
+      <c r="AV99" s="3"/>
+      <c r="AW99" s="3"/>
+      <c r="AX99" s="3"/>
+      <c r="AY99" s="3"/>
+      <c r="AZ99" s="3"/>
+      <c r="BA99" s="3"/>
+      <c r="BB99" s="3"/>
+      <c r="BC99" s="3"/>
+      <c r="BD99" s="3"/>
+      <c r="BE99" s="3"/>
+      <c r="BF99" s="3"/>
+      <c r="BG99" s="3"/>
+      <c r="BH99" s="3"/>
+      <c r="BI99" s="3"/>
+      <c r="BJ99" s="3"/>
+      <c r="BK99" s="3"/>
+      <c r="BL99" s="3"/>
+      <c r="BM99" s="3"/>
+      <c r="BN99" s="3"/>
+      <c r="BO99" s="3"/>
+      <c r="BP99" s="3"/>
+      <c r="BQ99" s="3"/>
+      <c r="BR99" s="3"/>
+      <c r="BS99" s="3"/>
+      <c r="BT99" s="3"/>
+      <c r="BU99" s="3"/>
+      <c r="BV99" s="3"/>
+      <c r="BW99" s="3"/>
+      <c r="BX99" s="3"/>
+      <c r="BY99" s="3"/>
+      <c r="BZ99" s="3"/>
+      <c r="CA99" s="3"/>
+      <c r="CB99" s="3"/>
+      <c r="CC99" s="3"/>
+      <c r="CD99" s="3"/>
+      <c r="CE99" s="3"/>
+      <c r="CF99" s="3"/>
+      <c r="CG99" s="3"/>
+      <c r="CH99" s="3"/>
+      <c r="CI99" s="3"/>
+      <c r="CM99" s="3"/>
+      <c r="CN99" s="3"/>
+    </row>
+    <row r="100" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="X100" s="3"/>
+      <c r="Y100" s="3"/>
+      <c r="Z100" s="3"/>
+      <c r="AA100" s="3"/>
+      <c r="AB100" s="3"/>
+      <c r="AC100" s="3"/>
+      <c r="AD100" s="3"/>
+      <c r="AE100" s="3"/>
+      <c r="AF100" s="3"/>
+      <c r="AG100" s="3"/>
+      <c r="AH100" s="3"/>
+      <c r="AI100" s="3"/>
+      <c r="AJ100" s="3"/>
+      <c r="AK100" s="3"/>
+      <c r="AL100" s="3"/>
+      <c r="AM100" s="3"/>
+      <c r="AN100" s="3"/>
+      <c r="AO100" s="3"/>
+      <c r="AP100" s="3"/>
+      <c r="AQ100" s="3"/>
+      <c r="AR100" s="3"/>
+      <c r="AS100" s="3"/>
+      <c r="AT100" s="3"/>
+      <c r="AU100" s="3"/>
+      <c r="AV100" s="3"/>
+      <c r="AW100" s="3"/>
+      <c r="AX100" s="3"/>
+      <c r="AY100" s="3"/>
+      <c r="AZ100" s="3"/>
+      <c r="BA100" s="3"/>
+      <c r="BB100" s="3"/>
+      <c r="BC100" s="3"/>
+      <c r="BD100" s="3"/>
+      <c r="BE100" s="3"/>
+      <c r="BF100" s="3"/>
+      <c r="BG100" s="3"/>
+      <c r="BH100" s="3"/>
+      <c r="BI100" s="3"/>
+      <c r="BJ100" s="3"/>
+      <c r="BK100" s="3"/>
+      <c r="BL100" s="3"/>
+      <c r="BM100" s="3"/>
+      <c r="BN100" s="3"/>
+      <c r="BO100" s="3"/>
+      <c r="BP100" s="3"/>
+      <c r="BQ100" s="3"/>
+      <c r="BR100" s="3"/>
+      <c r="BS100" s="3"/>
+      <c r="BT100" s="3"/>
+      <c r="BU100" s="3"/>
+      <c r="BV100" s="3"/>
+      <c r="BW100" s="3"/>
+      <c r="BX100" s="3"/>
+      <c r="BY100" s="3"/>
+      <c r="BZ100" s="3"/>
+      <c r="CA100" s="3"/>
+      <c r="CB100" s="3"/>
+      <c r="CC100" s="3"/>
+      <c r="CD100" s="3"/>
+      <c r="CE100" s="3"/>
+      <c r="CF100" s="3"/>
+      <c r="CG100" s="3"/>
+      <c r="CH100" s="3"/>
+      <c r="CI100" s="3"/>
+      <c r="CM100" s="3"/>
+      <c r="CN100" s="3"/>
+      <c r="CO100" s="3"/>
+    </row>
+    <row r="101" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="X101" s="3"/>
+      <c r="Y101" s="3"/>
+      <c r="Z101" s="3"/>
+      <c r="AA101" s="3"/>
+      <c r="AB101" s="3"/>
+      <c r="AC101" s="3"/>
+      <c r="AD101" s="3"/>
+      <c r="AE101" s="3"/>
+      <c r="AF101" s="3"/>
+      <c r="AG101" s="3"/>
+      <c r="AH101" s="3"/>
+      <c r="AI101" s="3"/>
+      <c r="AJ101" s="3"/>
+      <c r="AK101" s="3"/>
+      <c r="BF101" s="3"/>
+      <c r="BG101" s="3"/>
+      <c r="BH101" s="3"/>
+      <c r="BL101" s="3"/>
+      <c r="BP101" s="3"/>
+      <c r="BQ101" s="3"/>
+      <c r="BR101" s="3"/>
+      <c r="BS101" s="3"/>
+      <c r="BT101" s="3"/>
+      <c r="BU101" s="3"/>
+      <c r="BV101" s="3"/>
+      <c r="BW101" s="3"/>
+      <c r="BX101" s="3"/>
+      <c r="BY101" s="3"/>
+      <c r="BZ101" s="3"/>
+      <c r="CA101" s="3"/>
+      <c r="CB101" s="3"/>
+      <c r="CC101" s="3"/>
+      <c r="CD101" s="3"/>
+      <c r="CE101" s="3"/>
+      <c r="CF101" s="3"/>
+      <c r="CG101" s="3"/>
+      <c r="CH101" s="3"/>
+      <c r="CI101" s="3"/>
+      <c r="CM101" s="3"/>
+      <c r="CN101" s="3"/>
+      <c r="CO101" s="3"/>
+    </row>
+    <row r="102" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="X102" s="3"/>
+      <c r="Y102" s="3"/>
+      <c r="Z102" s="3"/>
+      <c r="AA102" s="3"/>
+      <c r="AB102" s="3"/>
+      <c r="AC102" s="3"/>
+      <c r="AD102" s="3"/>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="3"/>
+      <c r="AG102" s="3"/>
+      <c r="AH102" s="3"/>
+      <c r="AI102" s="3"/>
+      <c r="AJ102" s="3"/>
+      <c r="AK102" s="3"/>
+      <c r="BF102" s="3"/>
+      <c r="BG102" s="3"/>
+      <c r="BH102" s="3"/>
+      <c r="BL102" s="3"/>
+      <c r="BP102" s="3"/>
+      <c r="BQ102" s="3"/>
+      <c r="BR102" s="3"/>
+      <c r="BS102" s="3"/>
+      <c r="BT102" s="3"/>
+      <c r="BU102" s="3"/>
+      <c r="BV102" s="3"/>
+      <c r="BW102" s="3"/>
+      <c r="BX102" s="3"/>
+      <c r="BY102" s="3"/>
+      <c r="BZ102" s="3"/>
+      <c r="CA102" s="3"/>
+      <c r="CB102" s="3"/>
+      <c r="CC102" s="3"/>
+      <c r="CD102" s="3"/>
+      <c r="CE102" s="3"/>
+      <c r="CF102" s="3"/>
+      <c r="CG102" s="3"/>
+      <c r="CH102" s="3"/>
+      <c r="CI102" s="3"/>
+      <c r="CM102" s="3"/>
+      <c r="CN102" s="3"/>
+      <c r="CO102" s="3"/>
+    </row>
+    <row r="103" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="X103" s="3"/>
+      <c r="Y103" s="3"/>
+      <c r="Z103" s="3"/>
+      <c r="AA103" s="3"/>
+      <c r="AB103" s="3"/>
+      <c r="AC103" s="3"/>
+      <c r="AD103" s="3"/>
+      <c r="AE103" s="3"/>
+      <c r="AF103" s="3"/>
+      <c r="AG103" s="3"/>
+      <c r="AH103" s="3"/>
+      <c r="AI103" s="3"/>
+      <c r="AJ103" s="3"/>
+      <c r="AK103" s="3"/>
+      <c r="BF103" s="3"/>
+      <c r="BG103" s="3"/>
+      <c r="BH103" s="3"/>
+      <c r="BI103" s="3"/>
+      <c r="BL103" s="3"/>
+      <c r="BP103" s="3"/>
+      <c r="BQ103" s="3"/>
+      <c r="BR103" s="3"/>
+      <c r="BS103" s="3"/>
+      <c r="BT103" s="3"/>
+      <c r="BU103" s="3"/>
+      <c r="BV103" s="3"/>
+      <c r="BW103" s="3"/>
+      <c r="BX103" s="3"/>
+      <c r="BY103" s="3"/>
+      <c r="BZ103" s="3"/>
+      <c r="CA103" s="3"/>
+      <c r="CB103" s="3"/>
+      <c r="CC103" s="3"/>
+      <c r="CD103" s="3"/>
+      <c r="CE103" s="3"/>
+      <c r="CF103" s="3"/>
+      <c r="CG103" s="3"/>
+      <c r="CH103" s="3"/>
+      <c r="CI103" s="3"/>
+      <c r="CM103" s="3"/>
+      <c r="CN103" s="3"/>
+      <c r="CO103" s="3"/>
+    </row>
+    <row r="104" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="X104" s="3"/>
+      <c r="Y104" s="3"/>
+      <c r="Z104" s="3"/>
+      <c r="AA104" s="3"/>
+      <c r="AB104" s="3"/>
+      <c r="AC104" s="3"/>
+      <c r="AD104" s="3"/>
+      <c r="AE104" s="3"/>
+      <c r="AF104" s="3"/>
+      <c r="AG104" s="3"/>
+      <c r="AH104" s="3"/>
+      <c r="AI104" s="3"/>
+      <c r="AJ104" s="3"/>
+      <c r="AK104" s="15"/>
+      <c r="BF104" s="3"/>
+      <c r="BG104" s="3"/>
+      <c r="BH104" s="3"/>
+      <c r="BI104" s="3"/>
+      <c r="BL104" s="3"/>
+      <c r="BP104" s="3"/>
+      <c r="BQ104" s="3"/>
+      <c r="BR104" s="3"/>
+      <c r="BS104" s="3"/>
+      <c r="BT104" s="3"/>
+      <c r="BU104" s="3"/>
+      <c r="BV104" s="3"/>
+      <c r="BW104" s="3"/>
+      <c r="BX104" s="3"/>
+      <c r="BY104" s="3"/>
+      <c r="BZ104" s="3"/>
+      <c r="CA104" s="3"/>
+      <c r="CB104" s="3"/>
+      <c r="CC104" s="3"/>
+      <c r="CD104" s="3"/>
+      <c r="CE104" s="3"/>
+      <c r="CF104" s="3"/>
+      <c r="CG104" s="3"/>
+      <c r="CH104" s="3"/>
+      <c r="CI104" s="3"/>
+      <c r="CJ104" s="3"/>
+      <c r="CK104" s="3"/>
+      <c r="CL104" s="3"/>
+      <c r="CM104" s="3"/>
+      <c r="CN104" s="3"/>
+      <c r="CO104" s="3"/>
+    </row>
+    <row r="105" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="Y105" s="3"/>
+      <c r="Z105" s="3"/>
+      <c r="AA105" s="3"/>
+      <c r="AB105" s="3"/>
+      <c r="AC105" s="3"/>
+      <c r="AD105" s="3"/>
+      <c r="AE105" s="3"/>
+      <c r="AF105" s="3"/>
+      <c r="AG105" s="3"/>
+      <c r="AH105" s="3"/>
+      <c r="AI105" s="3"/>
+      <c r="AJ105" s="3"/>
+      <c r="AK105" s="3"/>
+      <c r="AL105" s="3"/>
+      <c r="AM105" s="3"/>
+      <c r="AN105" s="3"/>
+      <c r="AO105" s="3"/>
+      <c r="AP105" s="3"/>
+      <c r="AQ105" s="3"/>
+      <c r="AR105" s="3"/>
+      <c r="AS105" s="3"/>
+      <c r="AT105" s="3"/>
+      <c r="AU105" s="21"/>
+      <c r="AV105" s="21"/>
+      <c r="AW105" s="21"/>
+      <c r="AX105" s="21"/>
+      <c r="AY105" s="21"/>
+      <c r="AZ105" s="21"/>
+      <c r="BA105" s="21"/>
+      <c r="BB105" s="21"/>
+      <c r="BC105" s="21"/>
+      <c r="BD105" s="21"/>
+      <c r="BE105" s="21"/>
+      <c r="BF105" s="21"/>
+      <c r="BG105" s="21"/>
+      <c r="BH105" s="21"/>
+      <c r="BI105" s="3"/>
+      <c r="BJ105" s="3"/>
+      <c r="BK105" s="3"/>
+      <c r="BL105" s="3"/>
+      <c r="BM105" s="3"/>
+      <c r="BN105" s="3"/>
+      <c r="BO105" s="3"/>
+      <c r="BP105" s="3"/>
+      <c r="BQ105" s="3"/>
+      <c r="BR105" s="3"/>
+      <c r="BS105" s="3"/>
+      <c r="BT105" s="3"/>
+      <c r="BU105" s="3"/>
+      <c r="BV105" s="3"/>
+      <c r="BW105" s="3"/>
+      <c r="BX105" s="3"/>
+      <c r="BY105" s="3"/>
+      <c r="BZ105" s="3"/>
+      <c r="CA105" s="3"/>
+      <c r="CB105" s="5"/>
+      <c r="CC105" s="5"/>
+      <c r="CD105" s="5"/>
+      <c r="CE105" s="15"/>
+      <c r="CF105" s="3"/>
+      <c r="CG105" s="3"/>
+      <c r="CH105" s="3"/>
+      <c r="CI105" s="3"/>
+      <c r="CJ105" s="3"/>
+      <c r="CK105" s="3"/>
+      <c r="CL105" s="3"/>
+      <c r="CM105" s="3"/>
+      <c r="CN105" s="3"/>
+      <c r="CO105" s="3"/>
+    </row>
+    <row r="106" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="Y106" s="3"/>
+      <c r="Z106" s="3"/>
+      <c r="AA106" s="3"/>
+      <c r="AB106" s="3"/>
+      <c r="AC106" s="3"/>
+      <c r="AD106" s="3"/>
+      <c r="AE106" s="3"/>
+      <c r="AF106" s="3"/>
+      <c r="AG106" s="3"/>
+      <c r="AH106" s="3"/>
+      <c r="AI106" s="3"/>
+      <c r="AJ106" s="3"/>
+      <c r="AK106" s="3"/>
+      <c r="AL106" s="3"/>
+      <c r="AM106" s="3"/>
+      <c r="AN106" s="3"/>
+      <c r="AO106" s="3"/>
+      <c r="AP106" s="3"/>
+      <c r="AQ106" s="3"/>
+      <c r="AR106" s="3"/>
+      <c r="AS106" s="3"/>
+      <c r="AT106" s="3"/>
+      <c r="AU106" s="21"/>
+      <c r="AV106" s="21"/>
+      <c r="AW106" s="21"/>
+      <c r="AX106" s="21"/>
+      <c r="AY106" s="21"/>
+      <c r="AZ106" s="21"/>
+      <c r="BA106" s="21"/>
+      <c r="BB106" s="21"/>
+      <c r="BC106" s="21"/>
+      <c r="BD106" s="21"/>
+      <c r="BE106" s="21"/>
+      <c r="BF106" s="21"/>
+      <c r="BG106" s="21"/>
+      <c r="BH106" s="21"/>
+      <c r="BI106" s="3"/>
+      <c r="BJ106" s="3"/>
+      <c r="BK106" s="3"/>
+      <c r="BL106" s="3"/>
+      <c r="BM106" s="3"/>
+      <c r="BN106" s="3"/>
+      <c r="BO106" s="3"/>
+      <c r="BP106" s="3"/>
+      <c r="BQ106" s="3"/>
+      <c r="BR106" s="3"/>
+      <c r="BS106" s="3"/>
+      <c r="BT106" s="3"/>
+      <c r="BU106" s="3"/>
+      <c r="BV106" s="3"/>
+      <c r="BW106" s="3"/>
+      <c r="BX106" s="3"/>
+      <c r="BY106" s="3"/>
+      <c r="BZ106" s="3"/>
+      <c r="CA106" s="3"/>
+      <c r="CB106" s="3"/>
+      <c r="CC106" s="3"/>
+      <c r="CD106" s="3"/>
+      <c r="CE106" s="3"/>
+      <c r="CF106" s="3"/>
+      <c r="CG106" s="3"/>
+      <c r="CH106" s="3"/>
+      <c r="CI106" s="3"/>
+      <c r="CJ106" s="3"/>
+      <c r="CK106" s="3"/>
+      <c r="CL106" s="3"/>
+      <c r="CM106" s="3"/>
+      <c r="CN106" s="3"/>
+    </row>
+    <row r="107" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="Z107" s="3"/>
+      <c r="AA107" s="3"/>
+      <c r="AB107" s="3"/>
+      <c r="AC107" s="3"/>
+      <c r="AD107" s="3"/>
+      <c r="AE107" s="3"/>
+      <c r="AF107" s="3"/>
+      <c r="AG107" s="3"/>
+      <c r="AH107" s="3"/>
+      <c r="AI107" s="3"/>
+      <c r="AJ107" s="3"/>
+      <c r="AK107" s="3"/>
+      <c r="AU107" s="21"/>
+      <c r="AV107" s="21"/>
+      <c r="AW107" s="21"/>
+      <c r="AX107" s="21"/>
+      <c r="AY107" s="21"/>
+      <c r="AZ107" s="21"/>
+      <c r="BA107" s="21"/>
+      <c r="BB107" s="21"/>
+      <c r="BC107" s="21"/>
+      <c r="BD107" s="21"/>
+      <c r="BE107" s="21"/>
+      <c r="BF107" s="21"/>
+      <c r="BG107" s="21"/>
+      <c r="BH107" s="21"/>
+      <c r="BL107" s="3"/>
+      <c r="BP107" s="3"/>
+      <c r="BQ107" s="3"/>
+      <c r="BR107" s="3"/>
+      <c r="BS107" s="3"/>
+      <c r="BT107" s="3"/>
+      <c r="BU107" s="3"/>
+      <c r="BV107" s="3"/>
+      <c r="BW107" s="3"/>
+      <c r="BX107" s="3"/>
+      <c r="BY107" s="3"/>
+      <c r="BZ107" s="3"/>
+      <c r="CA107" s="3"/>
+      <c r="CB107" s="3"/>
+      <c r="CC107" s="3"/>
+      <c r="CD107" s="3"/>
+      <c r="CE107" s="3"/>
+      <c r="CF107" s="3"/>
+      <c r="CG107" s="3"/>
+      <c r="CH107" s="3"/>
+      <c r="CI107" s="3"/>
+      <c r="CJ107" s="3"/>
+      <c r="CK107" s="3"/>
+      <c r="CL107" s="3"/>
+      <c r="CM107" s="3"/>
+      <c r="CN107" s="3"/>
+    </row>
+    <row r="108" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="AG108" s="3"/>
+      <c r="AH108" s="3"/>
+      <c r="AI108" s="3"/>
+      <c r="AJ108" s="3"/>
+      <c r="AK108" s="3"/>
+      <c r="AU108" s="21"/>
+      <c r="AV108" s="21"/>
+      <c r="AW108" s="21"/>
+      <c r="AX108" s="21"/>
+      <c r="AY108" s="21"/>
+      <c r="AZ108" s="21"/>
+      <c r="BA108" s="21"/>
+      <c r="BB108" s="21"/>
+      <c r="BC108" s="21"/>
+      <c r="BD108" s="21"/>
+      <c r="BE108" s="21"/>
+      <c r="BF108" s="21"/>
+      <c r="BG108" s="21"/>
+      <c r="BH108" s="21"/>
+      <c r="BI108" s="3"/>
+      <c r="BJ108" s="3"/>
+      <c r="BK108" s="3"/>
+      <c r="BL108" s="3"/>
+      <c r="BM108" s="3"/>
+      <c r="BP108" s="3"/>
+      <c r="BQ108" s="3"/>
+      <c r="BR108" s="3"/>
+      <c r="BS108" s="3"/>
+      <c r="BT108" s="3"/>
+      <c r="BU108" s="3"/>
+      <c r="BV108" s="3"/>
+      <c r="BW108" s="3"/>
+      <c r="BX108" s="3"/>
+      <c r="BY108" s="3"/>
+      <c r="BZ108" s="3"/>
+      <c r="CA108" s="3"/>
+      <c r="CB108" s="3"/>
+      <c r="CC108" s="3"/>
+      <c r="CD108" s="3"/>
+      <c r="CE108" s="3"/>
+      <c r="CF108" s="3"/>
+      <c r="CG108" s="3"/>
+      <c r="CH108" s="3"/>
+      <c r="CI108" s="3"/>
+      <c r="CJ108" s="3"/>
+      <c r="CK108" s="3"/>
+      <c r="CL108" s="3"/>
+      <c r="CM108" s="3"/>
+      <c r="CN108" s="3"/>
+    </row>
+    <row r="109" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="AJ109" s="3"/>
+      <c r="AK109" s="3"/>
+      <c r="AU109" s="21"/>
+      <c r="AV109" s="21"/>
+      <c r="AW109" s="21"/>
+      <c r="AX109" s="21"/>
+      <c r="AY109" s="21"/>
+      <c r="AZ109" s="21"/>
+      <c r="BA109" s="21"/>
+      <c r="BB109" s="21"/>
+      <c r="BC109" s="21"/>
+      <c r="BD109" s="21"/>
+      <c r="BE109" s="21"/>
+      <c r="BF109" s="21"/>
+      <c r="BG109" s="21"/>
+      <c r="BH109" s="21"/>
+      <c r="BI109" s="3"/>
+      <c r="BJ109" s="3"/>
+      <c r="BK109" s="3"/>
+      <c r="BL109" s="3"/>
+      <c r="BM109" s="3"/>
+      <c r="BP109" s="3"/>
+      <c r="BQ109" s="3"/>
+      <c r="BR109" s="3"/>
+      <c r="BS109" s="3"/>
+      <c r="BT109" s="3"/>
+      <c r="BU109" s="3"/>
+      <c r="BV109" s="3"/>
+      <c r="BW109" s="3"/>
+      <c r="BX109" s="3"/>
+      <c r="BY109" s="3"/>
+      <c r="BZ109" s="3"/>
+      <c r="CA109" s="3"/>
+      <c r="CB109" s="3"/>
+      <c r="CC109" s="3"/>
+      <c r="CD109" s="3"/>
+      <c r="CE109" s="3"/>
+      <c r="CF109" s="3"/>
+      <c r="CG109" s="3"/>
+      <c r="CH109" s="3"/>
+      <c r="CI109" s="3"/>
+      <c r="CJ109" s="3"/>
+      <c r="CK109" s="3"/>
+      <c r="CL109" s="3"/>
+      <c r="CM109" s="3"/>
+      <c r="CN109" s="3"/>
+    </row>
+    <row r="110" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="AJ110" s="3"/>
+      <c r="AK110" s="3"/>
+      <c r="AU110" s="21"/>
+      <c r="AV110" s="21"/>
+      <c r="AW110" s="21"/>
+      <c r="AX110" s="21"/>
+      <c r="AY110" s="21"/>
+      <c r="AZ110" s="21"/>
+      <c r="BA110" s="21"/>
+      <c r="BB110" s="21"/>
+      <c r="BC110" s="21"/>
+      <c r="BD110" s="21"/>
+      <c r="BE110" s="21"/>
+      <c r="BF110" s="21"/>
+      <c r="BG110" s="21"/>
+      <c r="BH110" s="21"/>
+      <c r="BI110" s="3"/>
+      <c r="BJ110" s="3"/>
+      <c r="BK110" s="14"/>
+      <c r="BL110" s="14"/>
+      <c r="BM110" s="3"/>
+      <c r="BN110" s="3"/>
+      <c r="BO110" s="3"/>
+      <c r="BP110" s="3"/>
+      <c r="BQ110" s="3"/>
+      <c r="BR110" s="3"/>
+      <c r="BS110" s="3"/>
+      <c r="BT110" s="3"/>
+      <c r="BU110" s="3"/>
+      <c r="BV110" s="3"/>
+      <c r="BW110" s="3"/>
+      <c r="BX110" s="3"/>
+      <c r="BY110" s="3"/>
+      <c r="BZ110" s="3"/>
+      <c r="CA110" s="3"/>
+      <c r="CB110" s="3"/>
+      <c r="CC110" s="3"/>
+      <c r="CD110" s="3"/>
+      <c r="CE110" s="3"/>
+      <c r="CF110" s="3"/>
+      <c r="CG110" s="3"/>
+      <c r="CH110" s="3"/>
+      <c r="CI110" s="3"/>
+      <c r="CM110" s="3"/>
+      <c r="CN110" s="3"/>
+    </row>
+    <row r="111" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="AE111" s="16"/>
+      <c r="AF111" s="16"/>
+      <c r="AG111" s="16"/>
+      <c r="AH111" s="16"/>
+      <c r="AI111" s="16"/>
+      <c r="AJ111" s="16"/>
+      <c r="AK111" s="16"/>
+      <c r="AL111" s="16"/>
+      <c r="AU111" s="21"/>
+      <c r="AV111" s="21"/>
+      <c r="AW111" s="21"/>
+      <c r="AX111" s="21"/>
+      <c r="AY111" s="21"/>
+      <c r="AZ111" s="21"/>
+      <c r="BA111" s="21"/>
+      <c r="BB111" s="21"/>
+      <c r="BC111" s="21"/>
+      <c r="BD111" s="21"/>
+      <c r="BE111" s="21"/>
+      <c r="BF111" s="21"/>
+      <c r="BG111" s="21"/>
+      <c r="BH111" s="21"/>
+      <c r="BI111" s="3"/>
+      <c r="BJ111" s="3"/>
+      <c r="BK111" s="14"/>
+      <c r="BL111" s="14"/>
+      <c r="BM111" s="3"/>
+      <c r="BN111" s="3"/>
+      <c r="BO111" s="3"/>
+      <c r="BP111" s="3"/>
+      <c r="BQ111" s="3"/>
+      <c r="BR111" s="3"/>
+      <c r="BS111" s="3"/>
+      <c r="BT111" s="3"/>
+      <c r="BU111" s="3"/>
+      <c r="BV111" s="3"/>
+      <c r="BW111" s="3"/>
+      <c r="BX111" s="3"/>
+      <c r="BY111" s="3"/>
+      <c r="BZ111" s="3"/>
+      <c r="CA111" s="3"/>
+      <c r="CB111" s="3"/>
+      <c r="CC111" s="3"/>
+      <c r="CD111" s="3"/>
+      <c r="CE111" s="3"/>
+      <c r="CF111" s="3"/>
+      <c r="CG111" s="3"/>
+      <c r="CH111" s="3"/>
+      <c r="CI111" s="3"/>
+      <c r="CM111" s="3"/>
+      <c r="CN111" s="3"/>
+    </row>
+    <row r="112" spans="24:93" x14ac:dyDescent="0.2">
+      <c r="AJ112" s="3"/>
+      <c r="AU112" s="21"/>
+      <c r="AV112" s="21"/>
+      <c r="AW112" s="21"/>
+      <c r="AX112" s="21"/>
+      <c r="AY112" s="21"/>
+      <c r="AZ112" s="21"/>
+      <c r="BA112" s="21"/>
+      <c r="BB112" s="21"/>
+      <c r="BC112" s="21"/>
+      <c r="BD112" s="21"/>
+      <c r="BE112" s="21"/>
+      <c r="BF112" s="21"/>
+      <c r="BG112" s="21"/>
+      <c r="BH112" s="21"/>
+      <c r="BI112" s="3"/>
+      <c r="BJ112" s="3"/>
+      <c r="BK112" s="14"/>
+      <c r="BL112" s="14"/>
+      <c r="BQ112" s="3"/>
+      <c r="BS112" s="3"/>
+      <c r="BT112" s="3"/>
+      <c r="BU112" s="3"/>
+      <c r="BV112" s="3"/>
+      <c r="BW112" s="3"/>
+      <c r="BX112" s="3"/>
+      <c r="BY112" s="3"/>
+      <c r="BZ112" s="3"/>
+      <c r="CA112" s="3"/>
+      <c r="CB112" s="3"/>
+      <c r="CC112" s="3"/>
+      <c r="CD112" s="3"/>
+      <c r="CE112" s="3"/>
+      <c r="CF112" s="3"/>
+      <c r="CG112" s="3"/>
+      <c r="CH112" s="3"/>
+      <c r="CI112" s="3"/>
+      <c r="CJ112" s="3"/>
+      <c r="CK112" s="3"/>
+      <c r="CL112" s="3"/>
+      <c r="CM112" s="3"/>
+    </row>
+    <row r="113" spans="26:93" x14ac:dyDescent="0.2">
+      <c r="AJ113" s="3"/>
+      <c r="AU113" s="21"/>
+      <c r="AV113" s="21"/>
+      <c r="AW113" s="21"/>
+      <c r="AX113" s="21"/>
+      <c r="AY113" s="21"/>
+      <c r="AZ113" s="21"/>
+      <c r="BA113" s="21"/>
+      <c r="BB113" s="21"/>
+      <c r="BC113" s="21"/>
+      <c r="BD113" s="21"/>
+      <c r="BE113" s="21"/>
+      <c r="BF113" s="21"/>
+      <c r="BG113" s="21"/>
+      <c r="BH113" s="21"/>
+      <c r="BI113" s="3"/>
+      <c r="BJ113" s="3"/>
+      <c r="BL113" s="3"/>
+      <c r="BM113" s="3"/>
+      <c r="BN113" s="3"/>
+      <c r="BO113" s="3"/>
+      <c r="BQ113" s="3"/>
+      <c r="BS113" s="3"/>
+      <c r="BT113" s="3"/>
+      <c r="BU113" s="3"/>
+      <c r="BV113" s="3"/>
+      <c r="BW113" s="3"/>
+      <c r="BX113" s="3"/>
+      <c r="BY113" s="3"/>
+      <c r="BZ113" s="3"/>
+      <c r="CA113" s="3"/>
+      <c r="CB113" s="3"/>
+      <c r="CC113" s="3"/>
+      <c r="CD113" s="3"/>
+      <c r="CE113" s="3"/>
+      <c r="CF113" s="3"/>
+      <c r="CG113" s="3"/>
+      <c r="CH113" s="3"/>
+      <c r="CI113" s="3"/>
+      <c r="CJ113" s="3"/>
+      <c r="CK113" s="3"/>
+      <c r="CL113" s="3"/>
+      <c r="CM113" s="3"/>
+    </row>
+    <row r="114" spans="26:93" x14ac:dyDescent="0.2">
+      <c r="AJ114" s="3"/>
+      <c r="AK114" s="3"/>
+      <c r="AL114" s="3"/>
+      <c r="AM114" s="3"/>
+      <c r="AN114" s="3"/>
+      <c r="AO114" s="3"/>
+      <c r="AP114" s="3"/>
+      <c r="AQ114" s="3"/>
+      <c r="AR114" s="3"/>
+      <c r="AS114" s="3"/>
+      <c r="AT114" s="3"/>
+      <c r="AU114" s="3"/>
+      <c r="AV114" s="3"/>
+      <c r="AW114" s="3"/>
+      <c r="AX114" s="3"/>
+      <c r="AY114" s="3"/>
+      <c r="AZ114" s="3"/>
+      <c r="BA114" s="3"/>
+      <c r="BB114" s="3"/>
+      <c r="BC114" s="3"/>
+      <c r="BD114" s="3"/>
+      <c r="BE114" s="3"/>
+      <c r="BF114" s="3"/>
+      <c r="BG114" s="3"/>
+      <c r="BH114" s="3"/>
+      <c r="BI114" s="3"/>
+      <c r="BJ114" s="3"/>
+      <c r="BK114" s="3"/>
+      <c r="BL114" s="3"/>
+      <c r="BM114" s="3"/>
+      <c r="BQ114" s="3"/>
+      <c r="BS114" s="3"/>
+      <c r="BT114" s="3"/>
+      <c r="CG114" s="3"/>
+      <c r="CH114" s="3"/>
+      <c r="CI114" s="3"/>
+      <c r="CJ114" s="3"/>
+      <c r="CK114" s="3"/>
+      <c r="CL114" s="3"/>
+      <c r="CM114" s="3"/>
+      <c r="CN114" s="3"/>
+      <c r="CO114" s="3"/>
+    </row>
+    <row r="115" spans="26:93" x14ac:dyDescent="0.2">
+      <c r="AJ115" s="3"/>
+      <c r="AL115" s="3"/>
+      <c r="AM115" s="3"/>
+      <c r="AN115" s="3"/>
+      <c r="AO115" s="3"/>
+      <c r="AP115" s="3"/>
+      <c r="AQ115" s="3"/>
+      <c r="AR115" s="3"/>
+      <c r="AS115" s="3"/>
+      <c r="AT115" s="3"/>
+      <c r="AU115" s="3"/>
+      <c r="AV115" s="3"/>
+      <c r="AW115" s="3"/>
+      <c r="AX115" s="3"/>
+      <c r="AY115" s="3"/>
+      <c r="AZ115" s="3"/>
+      <c r="BA115" s="3"/>
+      <c r="BB115" s="3"/>
+      <c r="BC115" s="3"/>
+      <c r="BD115" s="3"/>
+      <c r="BE115" s="3"/>
+      <c r="BF115" s="3"/>
+      <c r="BG115" s="3"/>
+      <c r="BH115" s="3"/>
+      <c r="BI115" s="3"/>
+      <c r="BJ115" s="3"/>
+      <c r="BK115" s="3"/>
+      <c r="BL115" s="3"/>
+      <c r="BM115" s="3"/>
+      <c r="BN115" s="3"/>
+      <c r="BO115" s="3"/>
+      <c r="BP115" s="3"/>
+      <c r="BQ115" s="3"/>
+      <c r="BS115" s="3"/>
+      <c r="BT115" s="3"/>
+      <c r="CG115" s="3"/>
+      <c r="CH115" s="3"/>
+      <c r="CI115" s="3"/>
+      <c r="CJ115" s="3"/>
+      <c r="CK115" s="3"/>
+      <c r="CL115" s="3"/>
+      <c r="CM115" s="3"/>
+      <c r="CN115" s="3"/>
+      <c r="CO115" s="3"/>
+    </row>
+    <row r="116" spans="26:93" x14ac:dyDescent="0.2">
+      <c r="AJ116" s="3"/>
+      <c r="AR116" s="3"/>
+      <c r="AS116" s="3"/>
+      <c r="AT116" s="3"/>
+      <c r="AU116" s="3"/>
+      <c r="BB116" s="3"/>
+      <c r="BC116" s="3"/>
+      <c r="BD116" s="3"/>
+      <c r="BE116" s="3"/>
+      <c r="BF116" s="3"/>
+      <c r="BG116" s="3"/>
+      <c r="BH116" s="3"/>
+      <c r="BI116" s="3"/>
+      <c r="BJ116" s="3"/>
+      <c r="BK116" s="3"/>
+      <c r="BL116" s="3"/>
+      <c r="BM116" s="3"/>
+      <c r="BN116" s="3"/>
+      <c r="BO116" s="3"/>
+      <c r="BP116" s="3"/>
+      <c r="BQ116" s="3"/>
+      <c r="BS116" s="3"/>
+      <c r="BT116" s="3"/>
+      <c r="CG116" s="3"/>
+      <c r="CH116" s="3"/>
+      <c r="CI116" s="3"/>
+      <c r="CJ116" s="3"/>
+      <c r="CK116" s="3"/>
+      <c r="CL116" s="3"/>
+      <c r="CM116" s="3"/>
+      <c r="CN116" s="3"/>
+      <c r="CO116" s="3"/>
+    </row>
+    <row r="117" spans="26:93" x14ac:dyDescent="0.2">
+      <c r="AI117" s="16"/>
+      <c r="AJ117" s="16"/>
+      <c r="AK117" s="16"/>
+      <c r="AL117" s="16"/>
+      <c r="AM117" s="16"/>
+      <c r="AN117" s="16"/>
+      <c r="AO117" s="16"/>
+      <c r="AP117" s="16"/>
+      <c r="AQ117" s="16"/>
+      <c r="AR117" s="20"/>
+      <c r="AS117" s="3"/>
+      <c r="AT117" s="3"/>
+      <c r="AU117" s="3"/>
+      <c r="AV117" s="3"/>
+      <c r="AW117" s="3"/>
+      <c r="AX117" s="3"/>
+      <c r="AY117" s="3"/>
+      <c r="AZ117" s="3"/>
+      <c r="BA117" s="3"/>
+      <c r="BB117" s="3"/>
+      <c r="BC117" s="3"/>
+      <c r="BD117" s="3"/>
+      <c r="BE117" s="3"/>
+      <c r="BF117" s="3"/>
+      <c r="BG117" s="3"/>
+      <c r="BH117" s="3"/>
+      <c r="BI117" s="3"/>
+      <c r="BJ117" s="3"/>
+      <c r="BK117" s="3"/>
+      <c r="BL117" s="3"/>
+      <c r="BM117" s="3"/>
+      <c r="BN117" s="3"/>
+      <c r="BO117" s="3"/>
+      <c r="BP117" s="3"/>
+      <c r="BQ117" s="3"/>
+      <c r="BS117" s="3"/>
+      <c r="BT117" s="3"/>
+      <c r="CG117" s="3"/>
+      <c r="CH117" s="3"/>
+      <c r="CI117" s="3"/>
+      <c r="CJ117" s="3"/>
+      <c r="CK117" s="3"/>
+      <c r="CL117" s="3"/>
+      <c r="CM117" s="3"/>
+      <c r="CN117" s="3"/>
+      <c r="CO117" s="3"/>
+    </row>
+    <row r="118" spans="26:93" x14ac:dyDescent="0.2">
+      <c r="AI118" s="16"/>
+      <c r="AJ118" s="16"/>
+      <c r="AK118" s="16"/>
+      <c r="AL118" s="16"/>
+      <c r="AM118" s="16"/>
+      <c r="AN118" s="16"/>
+      <c r="AO118" s="16"/>
+      <c r="AP118" s="16"/>
+      <c r="AQ118" s="16"/>
+      <c r="AR118" s="20"/>
+      <c r="AS118" s="3"/>
+      <c r="AT118" s="3"/>
+      <c r="AU118" s="3"/>
+      <c r="AV118" s="3"/>
+      <c r="AW118" s="3"/>
+      <c r="AX118" s="3"/>
+      <c r="AY118" s="3"/>
+      <c r="AZ118" s="3"/>
+      <c r="BA118" s="3"/>
+      <c r="BB118" s="3"/>
+      <c r="BC118" s="3"/>
+      <c r="BD118" s="3"/>
+      <c r="BE118" s="3"/>
+      <c r="BF118" s="3"/>
+      <c r="BG118" s="3"/>
+      <c r="BH118" s="3"/>
+      <c r="BI118" s="3"/>
+      <c r="BJ118" s="3"/>
+      <c r="BK118" s="3"/>
+      <c r="BL118" s="3"/>
+      <c r="BM118" s="3"/>
+      <c r="BN118" s="3"/>
+      <c r="BO118" s="3"/>
+      <c r="BP118" s="3"/>
+      <c r="BQ118" s="3"/>
+      <c r="BR118" s="3"/>
+      <c r="BS118" s="3"/>
+      <c r="BT118" s="3"/>
+      <c r="BU118" s="3"/>
+      <c r="BV118" s="3"/>
+      <c r="BW118" s="3"/>
+      <c r="BX118" s="3"/>
+      <c r="BY118" s="3"/>
+      <c r="BZ118" s="3"/>
+      <c r="CA118" s="3"/>
+      <c r="CB118" s="3"/>
+      <c r="CC118" s="3"/>
+      <c r="CD118" s="3"/>
+      <c r="CE118" s="3"/>
+      <c r="CF118" s="3"/>
+      <c r="CG118" s="3"/>
+      <c r="CH118" s="3"/>
+      <c r="CI118" s="3"/>
+      <c r="CJ118" s="3"/>
+      <c r="CK118" s="3"/>
+      <c r="CL118" s="3"/>
+      <c r="CM118" s="3"/>
+      <c r="CN118" s="3"/>
+      <c r="CO118" s="3"/>
+    </row>
+    <row r="119" spans="26:93" x14ac:dyDescent="0.2">
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7"/>
+      <c r="AC119" s="7"/>
+      <c r="AD119" s="7"/>
+      <c r="AE119" s="7"/>
+      <c r="AI119" s="16"/>
+      <c r="AJ119" s="16"/>
+      <c r="AK119" s="16"/>
+      <c r="AL119" s="16"/>
+      <c r="AM119" s="16"/>
+      <c r="AN119" s="16"/>
+      <c r="AO119" s="16"/>
+      <c r="AP119" s="16"/>
+      <c r="AQ119" s="16"/>
+      <c r="AR119" s="3"/>
+      <c r="AS119" s="3"/>
+      <c r="AT119" s="3"/>
+      <c r="AU119" s="3"/>
+      <c r="AV119" s="3"/>
+      <c r="AW119" s="3"/>
+      <c r="AX119" s="3"/>
+      <c r="AY119" s="3"/>
+      <c r="AZ119" s="3"/>
+      <c r="BA119" s="3"/>
+      <c r="BB119" s="3"/>
+      <c r="BC119" s="3"/>
+      <c r="BD119" s="3"/>
+      <c r="BE119" s="3"/>
+      <c r="BF119" s="3"/>
+      <c r="BG119" s="3"/>
+      <c r="BH119" s="3"/>
+      <c r="BI119" s="3"/>
+      <c r="BJ119" s="3"/>
+      <c r="BK119" s="3"/>
+      <c r="BL119" s="3"/>
+      <c r="BM119" s="3"/>
+      <c r="BN119" s="3"/>
+      <c r="BO119" s="3"/>
+      <c r="BP119" s="3"/>
+      <c r="BQ119" s="3"/>
+      <c r="BS119" s="3"/>
+      <c r="BT119" s="3"/>
+    </row>
+    <row r="120" spans="26:93" x14ac:dyDescent="0.2">
+      <c r="Z120" s="13"/>
+      <c r="AA120" s="7"/>
+      <c r="AB120" s="7"/>
+      <c r="AC120" s="7"/>
+      <c r="AD120" s="7"/>
+      <c r="AE120" s="7"/>
+      <c r="AF120" s="7"/>
+      <c r="AP120" s="3"/>
+      <c r="AQ120" s="3"/>
+      <c r="AR120" s="3"/>
+      <c r="AS120" s="3"/>
+      <c r="AT120" s="3"/>
+      <c r="AU120" s="3"/>
+      <c r="AV120" s="3"/>
+      <c r="AW120" s="3"/>
+      <c r="AX120" s="3"/>
+      <c r="AY120" s="3"/>
+      <c r="AZ120" s="3"/>
+      <c r="BA120" s="3"/>
+      <c r="BB120" s="3"/>
+      <c r="BC120" s="3"/>
+      <c r="BD120" s="3"/>
+      <c r="BE120" s="3"/>
+      <c r="BF120" s="3"/>
+      <c r="BG120" s="3"/>
+      <c r="BH120" s="3"/>
+      <c r="BI120" s="3"/>
+      <c r="BJ120" s="3"/>
+      <c r="BK120" s="3"/>
+      <c r="BL120" s="3"/>
+      <c r="BM120" s="3"/>
+      <c r="BN120" s="3"/>
+      <c r="BO120" s="3"/>
+      <c r="BP120" s="3"/>
+      <c r="BQ120" s="3"/>
+      <c r="BR120" s="3"/>
+      <c r="BS120" s="3"/>
+      <c r="BT120" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="AI119:AQ119"/>
+    <mergeCell ref="M78:T78"/>
+    <mergeCell ref="AE111:AL111"/>
+    <mergeCell ref="AI117:AQ117"/>
+    <mergeCell ref="AI118:AQ118"/>
     <mergeCell ref="C17:H20"/>
     <mergeCell ref="F4:M4"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="F5:J5"/>
-    <mergeCell ref="H87:N87"/>
-    <mergeCell ref="I86:M86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
lives death system online poision gate layout complete and add some sounds!
</commit_message>
<xml_diff>
--- a/map_layout.xlsx
+++ b/map_layout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>=</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A 640 128</t>
+  </si>
+  <si>
+    <t>B 2176 128</t>
   </si>
 </sst>
 </file>
@@ -56,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +123,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -124,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -145,14 +169,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,87 +483,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:CO120"/>
+  <dimension ref="C1:DL120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y64" workbookViewId="0">
-      <selection activeCell="F86" sqref="F64:BY86"/>
+    <sheetView tabSelected="1" topLeftCell="AV33" workbookViewId="0">
+      <selection activeCell="BV42" sqref="BV37:CE42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.375" customWidth="1"/>
     <col min="5" max="5" width="2.375" customWidth="1"/>
+    <col min="79" max="88" width="2.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="4:106" x14ac:dyDescent="0.2">
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="4:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="4:106" x14ac:dyDescent="0.2">
       <c r="D2" s="4"/>
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
       <c r="S2" s="10"/>
     </row>
-    <row r="3" spans="4:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="4:106" x14ac:dyDescent="0.2">
       <c r="D3" s="2"/>
       <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
       <c r="S3" s="11"/>
     </row>
-    <row r="4" spans="4:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:106" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
       <c r="S4" s="9"/>
     </row>
-    <row r="5" spans="4:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="4:106" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="7" spans="4:45" x14ac:dyDescent="0.2">
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+    </row>
+    <row r="7" spans="4:106" x14ac:dyDescent="0.2">
       <c r="AI7" s="3"/>
-    </row>
-    <row r="12" spans="4:45" x14ac:dyDescent="0.2">
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="3"/>
+      <c r="AW7" s="3"/>
+      <c r="AX7" s="3"/>
+      <c r="AY7" s="3"/>
+      <c r="AZ7" s="3"/>
+      <c r="BA7" s="3"/>
+      <c r="BB7" s="3"/>
+      <c r="BC7" s="3"/>
+      <c r="BD7" s="3"/>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
+      <c r="BI7" s="3"/>
+      <c r="BJ7" s="3"/>
+      <c r="BK7" s="3"/>
+      <c r="BL7" s="3"/>
+      <c r="CF7" s="3"/>
+    </row>
+    <row r="8" spans="4:106" x14ac:dyDescent="0.2">
+      <c r="AU8" s="3"/>
+      <c r="AV8" s="3"/>
+      <c r="AW8" s="3"/>
+      <c r="AX8" s="3"/>
+      <c r="AY8" s="3"/>
+      <c r="AZ8" s="3"/>
+      <c r="BA8" s="3"/>
+      <c r="BB8" s="3"/>
+      <c r="BC8" s="3"/>
+      <c r="BD8" s="3"/>
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3"/>
+      <c r="BG8" s="3"/>
+      <c r="BH8" s="3"/>
+      <c r="BI8" s="3"/>
+      <c r="BJ8" s="3"/>
+      <c r="BK8" s="3"/>
+      <c r="BL8" s="3"/>
+      <c r="CF8" s="3"/>
+    </row>
+    <row r="9" spans="4:106" x14ac:dyDescent="0.2">
+      <c r="AU9" s="3"/>
+      <c r="AV9" s="3"/>
+      <c r="AW9" s="11"/>
+      <c r="AX9" s="11"/>
+      <c r="AY9" s="11"/>
+      <c r="AZ9" s="11"/>
+      <c r="BA9" s="11"/>
+      <c r="BB9" s="11"/>
+      <c r="BC9" s="11"/>
+      <c r="BD9" s="11"/>
+      <c r="BE9" s="11"/>
+      <c r="BF9" s="11"/>
+      <c r="BG9" s="11"/>
+      <c r="BH9" s="11"/>
+      <c r="BI9" s="11"/>
+      <c r="BJ9" s="11"/>
+      <c r="BK9" s="11"/>
+      <c r="BL9" s="11"/>
+      <c r="BM9" s="11"/>
+      <c r="BN9" s="11"/>
+      <c r="BO9" s="11"/>
+      <c r="BP9" s="11"/>
+      <c r="BQ9" s="11"/>
+      <c r="BR9" s="11"/>
+      <c r="BS9" s="11"/>
+      <c r="BT9" s="11"/>
+      <c r="BU9" s="11"/>
+      <c r="BV9" s="11"/>
+      <c r="BW9" s="11"/>
+      <c r="BX9" s="11"/>
+      <c r="BY9" s="11"/>
+      <c r="BZ9" s="11"/>
+      <c r="CA9" s="11"/>
+      <c r="CB9" s="11"/>
+      <c r="CC9" s="11"/>
+      <c r="CD9" s="11"/>
+      <c r="CE9" s="11"/>
+      <c r="CF9" s="11"/>
+      <c r="CG9" s="11"/>
+      <c r="CH9" s="11"/>
+      <c r="CI9" s="11"/>
+      <c r="CJ9" s="11"/>
+      <c r="CK9" s="11"/>
+      <c r="CL9" s="11"/>
+      <c r="CM9" s="11"/>
+      <c r="CN9" s="11"/>
+      <c r="CO9" s="11"/>
+      <c r="CP9" s="11"/>
+      <c r="CQ9" s="11"/>
+      <c r="CR9" s="11"/>
+      <c r="CS9" s="11"/>
+      <c r="CT9" s="11"/>
+      <c r="CU9" s="11"/>
+      <c r="CV9" s="11"/>
+      <c r="CW9" s="11"/>
+      <c r="CX9" s="11"/>
+      <c r="CY9" s="11"/>
+      <c r="CZ9" s="11"/>
+      <c r="DA9" s="11"/>
+      <c r="DB9" s="11"/>
+    </row>
+    <row r="10" spans="4:106" x14ac:dyDescent="0.2">
+      <c r="AU10" s="3"/>
+      <c r="AV10" s="3"/>
+      <c r="AW10" s="11"/>
+      <c r="AX10" s="11"/>
+      <c r="AY10" s="3"/>
+      <c r="AZ10" s="3"/>
+      <c r="BA10" s="3"/>
+      <c r="BB10" s="3"/>
+      <c r="BC10" s="3"/>
+      <c r="BD10" s="3"/>
+      <c r="BE10" s="3"/>
+      <c r="BF10" s="3"/>
+      <c r="BG10" s="3"/>
+      <c r="BH10" s="3"/>
+      <c r="BI10" s="11"/>
+      <c r="BJ10" s="3"/>
+      <c r="BK10" s="3"/>
+      <c r="BL10" s="3"/>
+      <c r="CF10" s="3"/>
+      <c r="DB10" s="11"/>
+    </row>
+    <row r="11" spans="4:106" x14ac:dyDescent="0.2">
+      <c r="AU11" s="3"/>
+      <c r="AV11" s="3"/>
+      <c r="AW11" s="11"/>
+      <c r="AX11" s="11"/>
+      <c r="AY11" s="3"/>
+      <c r="AZ11" s="3"/>
+      <c r="BA11" s="3"/>
+      <c r="BB11" s="3"/>
+      <c r="BC11" s="3"/>
+      <c r="BD11" s="3"/>
+      <c r="BE11" s="3"/>
+      <c r="BF11" s="3"/>
+      <c r="BG11" s="3"/>
+      <c r="BH11" s="3"/>
+      <c r="BI11" s="11"/>
+      <c r="BJ11" s="3"/>
+      <c r="BK11" s="3"/>
+      <c r="BL11" s="3"/>
+      <c r="CF11" s="3"/>
+      <c r="DB11" s="11"/>
+    </row>
+    <row r="12" spans="4:106" x14ac:dyDescent="0.2">
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -571,8 +747,49 @@
       <c r="AQ12" s="3"/>
       <c r="AR12" s="3"/>
       <c r="AS12" s="3"/>
-    </row>
-    <row r="13" spans="4:45" x14ac:dyDescent="0.2">
+      <c r="AU12" s="3"/>
+      <c r="AV12" s="3"/>
+      <c r="AW12" s="11"/>
+      <c r="AX12" s="11"/>
+      <c r="AY12" s="3"/>
+      <c r="AZ12" s="3"/>
+      <c r="BA12" s="3"/>
+      <c r="BB12" s="3"/>
+      <c r="BC12" s="3"/>
+      <c r="BD12" s="3"/>
+      <c r="BE12" s="3"/>
+      <c r="BF12" s="3"/>
+      <c r="BG12" s="3"/>
+      <c r="BH12" s="3"/>
+      <c r="BI12" s="11"/>
+      <c r="BJ12" s="3"/>
+      <c r="BK12" s="3"/>
+      <c r="BL12" s="3"/>
+      <c r="CC12" s="11"/>
+      <c r="CD12" s="2"/>
+      <c r="CE12" s="11"/>
+      <c r="CF12" s="2"/>
+      <c r="CG12" s="11"/>
+      <c r="CH12" s="2"/>
+      <c r="CI12" s="11"/>
+      <c r="CJ12" s="2"/>
+      <c r="CK12" s="11"/>
+      <c r="CL12" s="2"/>
+      <c r="CM12" s="11"/>
+      <c r="CN12" s="2"/>
+      <c r="CO12" s="11"/>
+      <c r="CP12" s="2"/>
+      <c r="CQ12" s="11"/>
+      <c r="CR12" s="2"/>
+      <c r="CS12" s="11"/>
+      <c r="CT12" s="2"/>
+      <c r="CU12" s="11"/>
+      <c r="CV12" s="2"/>
+      <c r="CW12" s="11"/>
+      <c r="CX12" s="2"/>
+      <c r="DB12" s="11"/>
+    </row>
+    <row r="13" spans="4:106" x14ac:dyDescent="0.2">
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -609,8 +826,25 @@
       <c r="AQ13" s="3"/>
       <c r="AR13" s="3"/>
       <c r="AS13" s="3"/>
-    </row>
-    <row r="14" spans="4:45" x14ac:dyDescent="0.2">
+      <c r="AW13" s="11"/>
+      <c r="AX13" s="11"/>
+      <c r="BB13" s="3"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3"/>
+      <c r="BI13" s="11"/>
+      <c r="BQ13" s="3"/>
+      <c r="BR13" s="3"/>
+      <c r="BS13" s="3"/>
+      <c r="BT13" s="3"/>
+      <c r="BU13" s="3"/>
+      <c r="BV13" s="3"/>
+      <c r="CB13" s="11"/>
+      <c r="CF13" s="3"/>
+      <c r="DB13" s="11"/>
+    </row>
+    <row r="14" spans="4:106" x14ac:dyDescent="0.2">
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -647,8 +881,40 @@
       <c r="AQ14" s="3"/>
       <c r="AR14" s="3"/>
       <c r="AS14" s="3"/>
-    </row>
-    <row r="15" spans="4:45" x14ac:dyDescent="0.2">
+      <c r="AW14" s="11"/>
+      <c r="AX14" s="11"/>
+      <c r="AY14" s="11"/>
+      <c r="AZ14" s="11"/>
+      <c r="BA14" s="11"/>
+      <c r="BB14" s="11"/>
+      <c r="BC14" s="11"/>
+      <c r="BD14" s="11"/>
+      <c r="BE14" s="11"/>
+      <c r="BF14" s="11"/>
+      <c r="BG14" s="11"/>
+      <c r="BH14" s="3"/>
+      <c r="BI14" s="11"/>
+      <c r="BJ14" s="11"/>
+      <c r="BK14" s="11"/>
+      <c r="BL14" s="11"/>
+      <c r="BM14" s="11"/>
+      <c r="BN14" s="11"/>
+      <c r="BO14" s="11"/>
+      <c r="BP14" s="11"/>
+      <c r="BR14" s="3"/>
+      <c r="BS14" s="11"/>
+      <c r="BT14" s="11"/>
+      <c r="BU14" s="11"/>
+      <c r="BV14" s="11"/>
+      <c r="BW14" s="11"/>
+      <c r="BX14" s="11"/>
+      <c r="BY14" s="11"/>
+      <c r="BZ14" s="11"/>
+      <c r="CA14" s="11"/>
+      <c r="CF14" s="3"/>
+      <c r="DB14" s="11"/>
+    </row>
+    <row r="15" spans="4:106" x14ac:dyDescent="0.2">
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -678,8 +944,21 @@
       <c r="AL15" s="1"/>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
-    </row>
-    <row r="16" spans="4:45" x14ac:dyDescent="0.2">
+      <c r="AW15" s="11"/>
+      <c r="AY15" s="3"/>
+      <c r="AZ15" s="3"/>
+      <c r="BA15" s="3"/>
+      <c r="BB15" s="3"/>
+      <c r="BC15" s="3"/>
+      <c r="BD15" s="3"/>
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3"/>
+      <c r="BG15" s="11"/>
+      <c r="BR15" s="11"/>
+      <c r="CF15" s="3"/>
+      <c r="DB15" s="11"/>
+    </row>
+    <row r="16" spans="4:106" x14ac:dyDescent="0.2">
       <c r="L16" s="1"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
@@ -687,14 +966,60 @@
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
       <c r="AN16" s="1"/>
-    </row>
-    <row r="17" spans="3:47" x14ac:dyDescent="0.2">
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="AW16" s="11"/>
+      <c r="AX16" s="3"/>
+      <c r="AY16" s="3"/>
+      <c r="AZ16" s="3"/>
+      <c r="BA16" s="3"/>
+      <c r="BB16" s="3"/>
+      <c r="BC16" s="3"/>
+      <c r="BD16" s="3"/>
+      <c r="BE16" s="3"/>
+      <c r="BF16" s="3"/>
+      <c r="BG16" s="11"/>
+      <c r="BQ16" s="11"/>
+      <c r="BU16" s="11"/>
+      <c r="BV16" s="11"/>
+      <c r="BW16" s="11"/>
+      <c r="BX16" s="11"/>
+      <c r="BY16" s="11"/>
+      <c r="BZ16" s="11"/>
+      <c r="CA16" s="11"/>
+      <c r="CB16" s="11"/>
+      <c r="CC16" s="11"/>
+      <c r="CD16" s="11"/>
+      <c r="CE16" s="11"/>
+      <c r="CF16" s="11"/>
+      <c r="CG16" s="11"/>
+      <c r="CH16" s="11"/>
+      <c r="CI16" s="11"/>
+      <c r="CJ16" s="11"/>
+      <c r="CK16" s="11"/>
+      <c r="CL16" s="11"/>
+      <c r="CM16" s="11"/>
+      <c r="CN16" s="11"/>
+      <c r="CO16" s="11"/>
+      <c r="CP16" s="11"/>
+      <c r="CQ16" s="11"/>
+      <c r="CR16" s="11"/>
+      <c r="CS16" s="11"/>
+      <c r="CT16" s="11"/>
+      <c r="CU16" s="11"/>
+      <c r="CV16" s="11"/>
+      <c r="CW16" s="11"/>
+      <c r="CX16" s="11"/>
+      <c r="CY16" s="11"/>
+      <c r="CZ16" s="11"/>
+      <c r="DA16" s="11"/>
+      <c r="DB16" s="11"/>
+    </row>
+    <row r="17" spans="3:106" x14ac:dyDescent="0.2">
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
       <c r="L17" s="1"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
@@ -702,14 +1027,28 @@
       <c r="AI17" s="3"/>
       <c r="AJ17" s="3"/>
       <c r="AN17" s="1"/>
-    </row>
-    <row r="18" spans="3:47" x14ac:dyDescent="0.2">
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="AW17" s="11"/>
+      <c r="AX17" s="3"/>
+      <c r="AY17" s="3"/>
+      <c r="AZ17" s="3"/>
+      <c r="BA17" s="3"/>
+      <c r="BB17" s="3"/>
+      <c r="BC17" s="3"/>
+      <c r="BD17" s="3"/>
+      <c r="BE17" s="3"/>
+      <c r="BF17" s="3"/>
+      <c r="BG17" s="11"/>
+      <c r="BP17" s="11"/>
+      <c r="CF17" s="3"/>
+      <c r="DB17" s="11"/>
+    </row>
+    <row r="18" spans="3:106" x14ac:dyDescent="0.2">
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
       <c r="L18" s="1"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
@@ -717,14 +1056,66 @@
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3"/>
       <c r="AN18" s="1"/>
-    </row>
-    <row r="19" spans="3:47" x14ac:dyDescent="0.2">
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="AW18" s="11"/>
+      <c r="AX18" s="3"/>
+      <c r="AY18" s="3"/>
+      <c r="AZ18" s="3"/>
+      <c r="BA18" s="3"/>
+      <c r="BB18" s="3"/>
+      <c r="BC18" s="3"/>
+      <c r="BD18" s="3"/>
+      <c r="BE18" s="3"/>
+      <c r="BF18" s="3"/>
+      <c r="BG18" s="11"/>
+      <c r="BI18" s="3"/>
+      <c r="BO18" s="11"/>
+      <c r="BP18" s="11"/>
+      <c r="BQ18" s="11"/>
+      <c r="BR18" s="11"/>
+      <c r="BS18" s="2"/>
+      <c r="BT18" s="11"/>
+      <c r="BU18" s="11"/>
+      <c r="BV18" s="11"/>
+      <c r="BW18" s="11"/>
+      <c r="BX18" s="11"/>
+      <c r="BY18" s="11"/>
+      <c r="BZ18" s="11"/>
+      <c r="CA18" s="11"/>
+      <c r="CB18" s="11"/>
+      <c r="CC18" s="11"/>
+      <c r="CD18" s="11"/>
+      <c r="CE18" s="11"/>
+      <c r="CF18" s="11"/>
+      <c r="CG18" s="11"/>
+      <c r="CH18" s="11"/>
+      <c r="CI18" s="11"/>
+      <c r="CJ18" s="3"/>
+      <c r="CK18" s="11"/>
+      <c r="CL18" s="11"/>
+      <c r="CM18" s="11"/>
+      <c r="CN18" s="11"/>
+      <c r="CO18" s="11"/>
+      <c r="CP18" s="11"/>
+      <c r="CQ18" s="11"/>
+      <c r="CR18" s="11"/>
+      <c r="CS18" s="11"/>
+      <c r="CT18" s="11"/>
+      <c r="CU18" s="11"/>
+      <c r="CV18" s="11"/>
+      <c r="CW18" s="11"/>
+      <c r="CX18" s="11"/>
+      <c r="CY18" s="11"/>
+      <c r="CZ18" s="11"/>
+      <c r="DA18" s="3"/>
+      <c r="DB18" s="11"/>
+    </row>
+    <row r="19" spans="3:106" x14ac:dyDescent="0.2">
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
       <c r="L19" s="1"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="1"/>
@@ -739,14 +1130,35 @@
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3"/>
       <c r="AN19" s="1"/>
-    </row>
-    <row r="20" spans="3:47" x14ac:dyDescent="0.2">
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="AW19" s="11"/>
+      <c r="AX19" s="3"/>
+      <c r="AY19" s="3"/>
+      <c r="AZ19" s="3"/>
+      <c r="BA19" s="3"/>
+      <c r="BB19" s="3"/>
+      <c r="BC19" s="3"/>
+      <c r="BD19" s="3"/>
+      <c r="BE19" s="3"/>
+      <c r="BF19" s="3"/>
+      <c r="BG19" s="11"/>
+      <c r="BH19" s="11"/>
+      <c r="BI19" s="3"/>
+      <c r="BJ19" s="11"/>
+      <c r="BK19" s="11"/>
+      <c r="BL19" s="11"/>
+      <c r="BM19" s="11"/>
+      <c r="BN19" s="11"/>
+      <c r="BO19" s="11"/>
+      <c r="CF19" s="3"/>
+      <c r="DB19" s="11"/>
+    </row>
+    <row r="20" spans="3:106" x14ac:dyDescent="0.2">
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="L20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="3"/>
@@ -764,8 +1176,22 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="2"/>
       <c r="AN20" s="1"/>
-    </row>
-    <row r="21" spans="3:47" x14ac:dyDescent="0.2">
+      <c r="AW20" s="11"/>
+      <c r="AX20" s="3"/>
+      <c r="AY20" s="3"/>
+      <c r="AZ20" s="3"/>
+      <c r="BA20" s="3"/>
+      <c r="BB20" s="3"/>
+      <c r="BC20" s="3"/>
+      <c r="BD20" s="3"/>
+      <c r="BE20" s="3"/>
+      <c r="BF20" s="3"/>
+      <c r="BG20" s="3"/>
+      <c r="BI20" s="3"/>
+      <c r="CF20" s="3"/>
+      <c r="DB20" s="11"/>
+    </row>
+    <row r="21" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L21" s="1"/>
       <c r="M21" s="12" t="s">
         <v>5</v>
@@ -787,8 +1213,66 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
       <c r="AN21" s="1"/>
-    </row>
-    <row r="22" spans="3:47" x14ac:dyDescent="0.2">
+      <c r="AW21" s="11"/>
+      <c r="AX21" s="11"/>
+      <c r="AY21" s="11"/>
+      <c r="AZ21" s="11"/>
+      <c r="BA21" s="11"/>
+      <c r="BB21" s="11"/>
+      <c r="BC21" s="11"/>
+      <c r="BD21" s="11"/>
+      <c r="BE21" s="11"/>
+      <c r="BF21" s="11"/>
+      <c r="BG21" s="11"/>
+      <c r="BH21" s="11"/>
+      <c r="BI21" s="3"/>
+      <c r="BJ21" s="11"/>
+      <c r="BK21" s="11"/>
+      <c r="BL21" s="11"/>
+      <c r="BM21" s="11"/>
+      <c r="BN21" s="11"/>
+      <c r="BO21" s="11"/>
+      <c r="BP21" s="11"/>
+      <c r="BQ21" s="11"/>
+      <c r="BR21" s="11"/>
+      <c r="BS21" s="11"/>
+      <c r="BT21" s="11"/>
+      <c r="BU21" s="11"/>
+      <c r="BV21" s="11"/>
+      <c r="BW21" s="11"/>
+      <c r="BX21" s="11"/>
+      <c r="BY21" s="11"/>
+      <c r="BZ21" s="11"/>
+      <c r="CA21" s="11"/>
+      <c r="CB21" s="11"/>
+      <c r="CC21" s="11"/>
+      <c r="CD21" s="11"/>
+      <c r="CE21" s="11"/>
+      <c r="CF21" s="11"/>
+      <c r="CG21" s="11"/>
+      <c r="CH21" s="11"/>
+      <c r="CI21" s="11"/>
+      <c r="CJ21" s="2"/>
+      <c r="CK21" s="11"/>
+      <c r="CL21" s="11"/>
+      <c r="CM21" s="11"/>
+      <c r="CN21" s="11"/>
+      <c r="CO21" s="11"/>
+      <c r="CP21" s="11"/>
+      <c r="CQ21" s="11"/>
+      <c r="CR21" s="11"/>
+      <c r="CS21" s="11"/>
+      <c r="CT21" s="11"/>
+      <c r="CU21" s="11"/>
+      <c r="CV21" s="11"/>
+      <c r="CW21" s="11"/>
+      <c r="CX21" s="11"/>
+      <c r="CY21" s="11"/>
+      <c r="CZ21" s="11"/>
+      <c r="DA21" s="11"/>
+      <c r="DB21" s="11"/>
+    </row>
+    <row r="22" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -813,8 +1297,13 @@
       <c r="AI22" s="3"/>
       <c r="AJ22" s="3"/>
       <c r="AN22" s="1"/>
-    </row>
-    <row r="23" spans="3:47" x14ac:dyDescent="0.2">
+      <c r="AV22" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI22" s="3"/>
+      <c r="CF22" s="3"/>
+    </row>
+    <row r="23" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L23" s="1"/>
       <c r="AB23" s="3"/>
       <c r="AF23" s="3"/>
@@ -824,7 +1313,7 @@
       <c r="AJ23" s="3"/>
       <c r="AN23" s="1"/>
     </row>
-    <row r="24" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L24" s="1"/>
       <c r="AB24" s="3"/>
       <c r="AF24" s="3"/>
@@ -834,7 +1323,7 @@
       <c r="AJ24" s="3"/>
       <c r="AN24" s="1"/>
     </row>
-    <row r="25" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -865,7 +1354,7 @@
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
     </row>
-    <row r="26" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L26" s="1"/>
       <c r="AB26" s="3"/>
       <c r="AI26" s="3"/>
@@ -874,7 +1363,7 @@
       <c r="AL26" s="3"/>
       <c r="AN26" s="1"/>
     </row>
-    <row r="27" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L27" s="1"/>
       <c r="AB27" s="3"/>
       <c r="AI27" s="3"/>
@@ -883,7 +1372,7 @@
       <c r="AL27" s="3"/>
       <c r="AN27" s="1"/>
     </row>
-    <row r="28" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -921,7 +1410,7 @@
       <c r="AT28" s="1"/>
       <c r="AU28" s="1"/>
     </row>
-    <row r="29" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L29" s="1"/>
       <c r="AI29" s="3"/>
       <c r="AJ29" s="3"/>
@@ -930,7 +1419,7 @@
       <c r="AN29" s="1"/>
       <c r="AU29" s="1"/>
     </row>
-    <row r="30" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:106" x14ac:dyDescent="0.2">
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -945,7 +1434,7 @@
       <c r="AQ30" s="1"/>
       <c r="AU30" s="1"/>
     </row>
-    <row r="31" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L31" s="1"/>
       <c r="M31" s="3"/>
       <c r="N31" s="1"/>
@@ -979,7 +1468,7 @@
       <c r="AS31" s="1"/>
       <c r="AU31" s="1"/>
     </row>
-    <row r="32" spans="3:47" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:106" x14ac:dyDescent="0.2">
       <c r="L32" s="1"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
@@ -999,7 +1488,7 @@
       <c r="AS32" s="1"/>
       <c r="AU32" s="1"/>
     </row>
-    <row r="33" spans="12:47" x14ac:dyDescent="0.2">
+    <row r="33" spans="12:116" x14ac:dyDescent="0.2">
       <c r="L33" s="1"/>
       <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
@@ -1018,8 +1507,15 @@
       <c r="AR33" s="1"/>
       <c r="AS33" s="1"/>
       <c r="AU33" s="1"/>
-    </row>
-    <row r="34" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="CO33" s="3"/>
+      <c r="CP33" s="3"/>
+      <c r="CQ33" s="3"/>
+      <c r="CR33" s="3"/>
+      <c r="CS33" s="3"/>
+      <c r="CT33" s="3"/>
+      <c r="CU33" s="3"/>
+    </row>
+    <row r="34" spans="12:116" x14ac:dyDescent="0.2">
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -1055,8 +1551,34 @@
       <c r="AR34" s="1"/>
       <c r="AS34" s="1"/>
       <c r="AU34" s="1"/>
-    </row>
-    <row r="35" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="BV34" s="22"/>
+      <c r="BW34" s="22"/>
+      <c r="BX34" s="22"/>
+      <c r="BY34" s="22"/>
+      <c r="BZ34" s="22"/>
+      <c r="CA34" s="22"/>
+      <c r="CB34" s="22"/>
+      <c r="CC34" s="22"/>
+      <c r="CD34" s="22"/>
+      <c r="CE34" s="22"/>
+      <c r="CF34" s="22"/>
+      <c r="CG34" s="22"/>
+      <c r="CH34" s="22"/>
+      <c r="CI34" s="22"/>
+      <c r="CJ34" s="22"/>
+      <c r="CK34" s="22"/>
+      <c r="CL34" s="22"/>
+      <c r="CM34" s="22"/>
+      <c r="CN34" s="22"/>
+      <c r="CO34" s="22"/>
+      <c r="CP34" s="22"/>
+      <c r="CQ34" s="3"/>
+      <c r="CR34" s="3"/>
+      <c r="CS34" s="3"/>
+      <c r="CT34" s="3"/>
+      <c r="CU34" s="3"/>
+    </row>
+    <row r="35" spans="12:116" x14ac:dyDescent="0.2">
       <c r="R35" s="1"/>
       <c r="T35" s="1"/>
       <c r="W35" s="1"/>
@@ -1082,8 +1604,18 @@
       <c r="AQ35" s="3"/>
       <c r="AR35" s="3"/>
       <c r="AU35" s="1"/>
-    </row>
-    <row r="36" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="BV35" s="22"/>
+      <c r="BX35" s="3"/>
+      <c r="CN35" s="3"/>
+      <c r="CO35" s="3"/>
+      <c r="CP35" s="22"/>
+      <c r="CQ35" s="3"/>
+      <c r="CR35" s="3"/>
+      <c r="CS35" s="3"/>
+      <c r="CT35" s="3"/>
+      <c r="CU35" s="3"/>
+    </row>
+    <row r="36" spans="12:116" x14ac:dyDescent="0.2">
       <c r="R36" s="1"/>
       <c r="T36" s="1"/>
       <c r="W36" s="1"/>
@@ -1109,8 +1641,41 @@
       <c r="AQ36" s="3"/>
       <c r="AR36" s="3"/>
       <c r="AU36" s="1"/>
-    </row>
-    <row r="37" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="AZ36" s="3"/>
+      <c r="BA36" s="3"/>
+      <c r="BB36" s="3"/>
+      <c r="BC36" s="3"/>
+      <c r="BD36" s="3"/>
+      <c r="BE36" s="3"/>
+      <c r="BF36" s="3"/>
+      <c r="BG36" s="3"/>
+      <c r="BH36" s="3"/>
+      <c r="BI36" s="3"/>
+      <c r="BJ36" s="3"/>
+      <c r="BK36" s="3"/>
+      <c r="BL36" s="3"/>
+      <c r="BM36" s="3"/>
+      <c r="BN36" s="3"/>
+      <c r="BO36" s="3"/>
+      <c r="BP36" s="3"/>
+      <c r="BQ36" s="3"/>
+      <c r="BR36" s="3"/>
+      <c r="BS36" s="3"/>
+      <c r="BT36" s="3"/>
+      <c r="BU36" s="3"/>
+      <c r="BV36" s="22"/>
+      <c r="BW36" s="3"/>
+      <c r="BX36" s="3"/>
+      <c r="CN36" s="3"/>
+      <c r="CO36" s="3"/>
+      <c r="CP36" s="22"/>
+      <c r="CQ36" s="3"/>
+      <c r="CR36" s="3"/>
+      <c r="CS36" s="3"/>
+      <c r="CT36" s="3"/>
+      <c r="CU36" s="3"/>
+    </row>
+    <row r="37" spans="12:116" x14ac:dyDescent="0.2">
       <c r="R37" s="1"/>
       <c r="T37" s="1"/>
       <c r="W37" s="1"/>
@@ -1138,8 +1703,41 @@
       <c r="AS37" s="3"/>
       <c r="AT37" s="3"/>
       <c r="AU37" s="1"/>
-    </row>
-    <row r="38" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="AZ37" s="3"/>
+      <c r="BA37" s="3"/>
+      <c r="BB37" s="3"/>
+      <c r="BC37" s="3"/>
+      <c r="BD37" s="3"/>
+      <c r="BE37" s="3"/>
+      <c r="BF37" s="3"/>
+      <c r="BG37" s="3"/>
+      <c r="BH37" s="3"/>
+      <c r="BI37" s="3"/>
+      <c r="BJ37" s="3"/>
+      <c r="BK37" s="3"/>
+      <c r="BL37" s="3"/>
+      <c r="BM37" s="3"/>
+      <c r="BN37" s="3"/>
+      <c r="BO37" s="3"/>
+      <c r="BP37" s="3"/>
+      <c r="BQ37" s="3"/>
+      <c r="BR37" s="3"/>
+      <c r="BS37" s="3"/>
+      <c r="BT37" s="3"/>
+      <c r="BU37" s="3"/>
+      <c r="BV37" s="22"/>
+      <c r="BW37" s="3"/>
+      <c r="BX37" s="3"/>
+      <c r="CN37" s="3"/>
+      <c r="CO37" s="3"/>
+      <c r="CP37" s="22"/>
+      <c r="CQ37" s="3"/>
+      <c r="CR37" s="3"/>
+      <c r="CS37" s="3"/>
+      <c r="CT37" s="3"/>
+      <c r="CU37" s="3"/>
+    </row>
+    <row r="38" spans="12:116" x14ac:dyDescent="0.2">
       <c r="R38" s="1"/>
       <c r="T38" s="1"/>
       <c r="W38" s="1"/>
@@ -1167,8 +1765,73 @@
       <c r="AS38" s="3"/>
       <c r="AT38" s="3"/>
       <c r="AU38" s="1"/>
-    </row>
-    <row r="39" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="AZ38" s="3"/>
+      <c r="BA38" s="3"/>
+      <c r="BB38" s="3"/>
+      <c r="BC38" s="3"/>
+      <c r="BD38" s="3"/>
+      <c r="BE38" s="3"/>
+      <c r="BF38" s="3"/>
+      <c r="BG38" s="3"/>
+      <c r="BH38" s="3"/>
+      <c r="BI38" s="3"/>
+      <c r="BJ38" s="3"/>
+      <c r="BK38" s="3"/>
+      <c r="BL38" s="3"/>
+      <c r="BM38" s="3"/>
+      <c r="BN38" s="3"/>
+      <c r="BO38" s="3"/>
+      <c r="BP38" s="3"/>
+      <c r="BQ38" s="3"/>
+      <c r="BR38" s="3"/>
+      <c r="BS38" s="3"/>
+      <c r="BT38" s="3"/>
+      <c r="BU38" s="3"/>
+      <c r="BV38" s="22"/>
+      <c r="BW38" s="22"/>
+      <c r="BX38" s="22"/>
+      <c r="BY38" s="22"/>
+      <c r="BZ38" s="23"/>
+      <c r="CA38" s="23"/>
+      <c r="CB38" s="3"/>
+      <c r="CC38" s="3"/>
+      <c r="CD38" s="23"/>
+      <c r="CE38" s="23"/>
+      <c r="CF38" s="23"/>
+      <c r="CG38" s="23"/>
+      <c r="CH38" s="23"/>
+      <c r="CI38" s="3"/>
+      <c r="CJ38" s="3"/>
+      <c r="CK38" s="23"/>
+      <c r="CL38" s="23"/>
+      <c r="CM38" s="22"/>
+      <c r="CN38" s="22"/>
+      <c r="CO38" s="22"/>
+      <c r="CP38" s="22"/>
+      <c r="CQ38" s="3"/>
+      <c r="CR38" s="3"/>
+      <c r="CS38" s="3"/>
+      <c r="CT38" s="3"/>
+      <c r="CU38" s="3"/>
+      <c r="CV38" s="3"/>
+      <c r="CW38" s="3"/>
+      <c r="CX38" s="3"/>
+      <c r="CY38" s="3"/>
+      <c r="CZ38" s="3"/>
+      <c r="DA38" s="3"/>
+      <c r="DB38" s="3"/>
+      <c r="DC38" s="3"/>
+      <c r="DD38" s="3"/>
+      <c r="DE38" s="3"/>
+      <c r="DF38" s="3"/>
+      <c r="DG38" s="3"/>
+      <c r="DH38" s="3"/>
+      <c r="DI38" s="3"/>
+      <c r="DJ38" s="3"/>
+      <c r="DK38" s="3"/>
+      <c r="DL38" s="3"/>
+    </row>
+    <row r="39" spans="12:116" x14ac:dyDescent="0.2">
       <c r="R39" s="1"/>
       <c r="T39" s="1"/>
       <c r="W39" s="1"/>
@@ -1196,8 +1859,44 @@
       <c r="AS39" s="3"/>
       <c r="AT39" s="3"/>
       <c r="AU39" s="1"/>
-    </row>
-    <row r="40" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="AZ39" s="3"/>
+      <c r="BA39" s="3"/>
+      <c r="BB39" s="3"/>
+      <c r="BC39" s="3"/>
+      <c r="BD39" s="3"/>
+      <c r="BE39" s="3"/>
+      <c r="BF39" s="3"/>
+      <c r="BG39" s="3"/>
+      <c r="BH39" s="3"/>
+      <c r="BI39" s="3"/>
+      <c r="BJ39" s="3"/>
+      <c r="BK39" s="3"/>
+      <c r="BL39" s="3"/>
+      <c r="BM39" s="3"/>
+      <c r="BN39" s="3"/>
+      <c r="BO39" s="3"/>
+      <c r="BP39" s="3"/>
+      <c r="BQ39" s="3"/>
+      <c r="BR39" s="3"/>
+      <c r="BS39" s="3"/>
+      <c r="BT39" s="3"/>
+      <c r="BU39" s="3"/>
+      <c r="BV39" s="22"/>
+      <c r="BW39" s="3"/>
+      <c r="BX39" s="3"/>
+      <c r="CC39" s="23"/>
+      <c r="CI39" s="22"/>
+      <c r="CN39" s="3"/>
+      <c r="CO39" s="3"/>
+      <c r="CP39" s="22"/>
+      <c r="CQ39" s="3"/>
+      <c r="CR39" s="3"/>
+      <c r="CS39" s="3"/>
+      <c r="CT39" s="3"/>
+      <c r="CU39" s="3"/>
+      <c r="DL39" s="3"/>
+    </row>
+    <row r="40" spans="12:116" x14ac:dyDescent="0.2">
       <c r="R40" s="1"/>
       <c r="T40" s="1"/>
       <c r="W40" s="1"/>
@@ -1225,34 +1924,670 @@
       <c r="AS40" s="2"/>
       <c r="AT40" s="1"/>
       <c r="AU40" s="1"/>
-    </row>
-    <row r="41" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="AZ40" s="3"/>
+      <c r="BA40" s="3"/>
+      <c r="BB40" s="3"/>
+      <c r="BC40" s="3"/>
+      <c r="BD40" s="3"/>
+      <c r="BE40" s="3"/>
+      <c r="BF40" s="3"/>
+      <c r="BG40" s="3"/>
+      <c r="BH40" s="3"/>
+      <c r="BI40" s="3"/>
+      <c r="BJ40" s="3"/>
+      <c r="BK40" s="3"/>
+      <c r="BL40" s="3"/>
+      <c r="BM40" s="3"/>
+      <c r="BN40" s="3"/>
+      <c r="BO40" s="3"/>
+      <c r="BP40" s="3"/>
+      <c r="BQ40" s="3"/>
+      <c r="BR40" s="3"/>
+      <c r="BS40" s="3"/>
+      <c r="BT40" s="3"/>
+      <c r="BU40" s="3"/>
+      <c r="BV40" s="22"/>
+      <c r="BW40" s="3"/>
+      <c r="BX40" s="3"/>
+      <c r="CB40" s="23"/>
+      <c r="CJ40" s="22"/>
+      <c r="CN40" s="3"/>
+      <c r="CO40" s="3"/>
+      <c r="CP40" s="22"/>
+      <c r="CQ40" s="3"/>
+      <c r="CR40" s="3"/>
+      <c r="CS40" s="3"/>
+      <c r="CT40" s="3"/>
+      <c r="CU40" s="3"/>
+      <c r="DL40" s="3"/>
+    </row>
+    <row r="41" spans="12:116" x14ac:dyDescent="0.2">
       <c r="R41" s="1"/>
       <c r="T41" s="1"/>
       <c r="AI41" s="3"/>
-    </row>
-    <row r="42" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="AZ41" s="3"/>
+      <c r="BA41" s="3"/>
+      <c r="BB41" s="3"/>
+      <c r="BC41" s="3"/>
+      <c r="BD41" s="3"/>
+      <c r="BE41" s="3"/>
+      <c r="BF41" s="3"/>
+      <c r="BG41" s="3"/>
+      <c r="BH41" s="3"/>
+      <c r="BI41" s="3"/>
+      <c r="BJ41" s="3"/>
+      <c r="BK41" s="3"/>
+      <c r="BL41" s="3"/>
+      <c r="BM41" s="3"/>
+      <c r="BN41" s="3"/>
+      <c r="BO41" s="3"/>
+      <c r="BP41" s="3"/>
+      <c r="BQ41" s="3"/>
+      <c r="BR41" s="3"/>
+      <c r="BS41" s="3"/>
+      <c r="BT41" s="3"/>
+      <c r="BU41" s="3"/>
+      <c r="BV41" s="22"/>
+      <c r="BW41" s="3"/>
+      <c r="BX41" s="3"/>
+      <c r="BY41" s="3"/>
+      <c r="BZ41" s="3"/>
+      <c r="CA41" s="22"/>
+      <c r="CB41" s="3"/>
+      <c r="CC41" s="3"/>
+      <c r="CD41" s="3"/>
+      <c r="CE41" s="3"/>
+      <c r="CK41" s="22"/>
+      <c r="CM41" s="3"/>
+      <c r="CN41" s="3"/>
+      <c r="CO41" s="3"/>
+      <c r="CP41" s="22"/>
+      <c r="CQ41" s="3"/>
+      <c r="CR41" s="3"/>
+      <c r="CS41" s="3"/>
+      <c r="CT41" s="3"/>
+      <c r="CU41" s="3"/>
+      <c r="CV41" s="3"/>
+      <c r="CW41" s="3"/>
+      <c r="CX41" s="3"/>
+      <c r="CY41" s="3"/>
+      <c r="CZ41" s="3"/>
+      <c r="DA41" s="3"/>
+      <c r="DB41" s="3"/>
+      <c r="DC41" s="3"/>
+      <c r="DD41" s="3"/>
+      <c r="DE41" s="3"/>
+      <c r="DF41" s="3"/>
+      <c r="DG41" s="3"/>
+      <c r="DH41" s="3"/>
+      <c r="DL41" s="3"/>
+    </row>
+    <row r="42" spans="12:116" x14ac:dyDescent="0.2">
       <c r="R42" s="1"/>
       <c r="S42" s="3"/>
       <c r="T42" s="1"/>
       <c r="AI42" s="3"/>
-    </row>
-    <row r="43" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="AZ42" s="3"/>
+      <c r="BA42" s="3"/>
+      <c r="BB42" s="3"/>
+      <c r="BC42" s="3"/>
+      <c r="BD42" s="3"/>
+      <c r="BE42" s="3"/>
+      <c r="BF42" s="3"/>
+      <c r="BG42" s="3"/>
+      <c r="BH42" s="3"/>
+      <c r="BI42" s="3"/>
+      <c r="BJ42" s="3"/>
+      <c r="BK42" s="3"/>
+      <c r="BL42" s="3"/>
+      <c r="BM42" s="3"/>
+      <c r="BN42" s="3"/>
+      <c r="BO42" s="3"/>
+      <c r="BP42" s="3"/>
+      <c r="BQ42" s="3"/>
+      <c r="BR42" s="3"/>
+      <c r="BS42" s="3"/>
+      <c r="BT42" s="3"/>
+      <c r="BU42" s="3"/>
+      <c r="BV42" s="22"/>
+      <c r="BW42" s="22"/>
+      <c r="BX42" s="22"/>
+      <c r="BY42" s="22"/>
+      <c r="BZ42" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA42" s="22"/>
+      <c r="CB42" s="22"/>
+      <c r="CC42" s="22"/>
+      <c r="CD42" s="22"/>
+      <c r="CE42" s="22"/>
+      <c r="CF42" s="22"/>
+      <c r="CG42" s="22"/>
+      <c r="CH42" s="22"/>
+      <c r="CI42" s="22"/>
+      <c r="CJ42" s="22"/>
+      <c r="CK42" s="22"/>
+      <c r="CL42" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="CM42" s="22"/>
+      <c r="CN42" s="22"/>
+      <c r="CO42" s="22"/>
+      <c r="CP42" s="22"/>
+      <c r="CQ42" s="3"/>
+      <c r="CR42" s="3"/>
+      <c r="CS42" s="3"/>
+      <c r="CT42" s="3"/>
+      <c r="CU42" s="3"/>
+      <c r="DL42" s="3"/>
+    </row>
+    <row r="43" spans="12:116" x14ac:dyDescent="0.2">
       <c r="L43" t="s">
         <v>1</v>
       </c>
       <c r="AI43" s="3"/>
-    </row>
-    <row r="44" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="AZ43" s="3"/>
+      <c r="BA43" s="3"/>
+      <c r="BB43" s="3"/>
+      <c r="BC43" s="3"/>
+      <c r="BD43" s="3"/>
+      <c r="BE43" s="3"/>
+      <c r="BF43" s="3"/>
+      <c r="BG43" s="3"/>
+      <c r="BH43" s="3"/>
+      <c r="BI43" s="3"/>
+      <c r="BJ43" s="3"/>
+      <c r="BK43" s="3"/>
+      <c r="BL43" s="3"/>
+      <c r="BM43" s="3"/>
+      <c r="BN43" s="3"/>
+      <c r="BO43" s="3"/>
+      <c r="BP43" s="3"/>
+      <c r="BQ43" s="3"/>
+      <c r="BR43" s="3"/>
+      <c r="BS43" s="3"/>
+      <c r="BT43" s="3"/>
+      <c r="BU43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BV43" s="3"/>
+      <c r="BW43" s="3"/>
+      <c r="BX43" s="3"/>
+      <c r="BY43" s="3"/>
+      <c r="BZ43" s="3"/>
+      <c r="CA43" s="3"/>
+      <c r="CB43" s="3"/>
+      <c r="CC43" s="3"/>
+      <c r="CD43" s="3"/>
+      <c r="CE43" s="3"/>
+      <c r="CO43" s="3"/>
+      <c r="CP43" s="3"/>
+      <c r="CQ43" s="3"/>
+      <c r="CR43" s="3"/>
+      <c r="CS43" s="3"/>
+      <c r="CT43" s="3"/>
+      <c r="CU43" s="3"/>
+      <c r="DL43" s="3"/>
+    </row>
+    <row r="44" spans="12:116" x14ac:dyDescent="0.2">
       <c r="AI44" s="3"/>
-    </row>
-    <row r="45" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="BC44" s="3"/>
+      <c r="BD44" s="3"/>
+      <c r="BE44" s="3"/>
+      <c r="BF44" s="3"/>
+      <c r="BG44" s="3"/>
+      <c r="BH44" s="3"/>
+      <c r="BI44" s="3"/>
+      <c r="BJ44" s="3"/>
+      <c r="BK44" s="3"/>
+      <c r="BL44" s="3"/>
+      <c r="BM44" s="3"/>
+      <c r="BN44" s="3"/>
+      <c r="BO44" s="3"/>
+      <c r="BP44" s="3"/>
+      <c r="BQ44" s="3"/>
+      <c r="BR44" s="3"/>
+      <c r="BS44" s="3"/>
+      <c r="BT44" s="3"/>
+      <c r="BU44" s="3"/>
+      <c r="BV44" s="3"/>
+      <c r="BW44" s="3"/>
+      <c r="BY44" s="3"/>
+      <c r="BZ44" s="3"/>
+      <c r="CA44" s="3"/>
+      <c r="CB44" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="CC44" s="24"/>
+      <c r="CD44" s="24"/>
+      <c r="CE44" s="24"/>
+      <c r="CF44" s="24"/>
+      <c r="CO44" s="3"/>
+      <c r="CP44" s="3"/>
+      <c r="CQ44" s="3"/>
+      <c r="CR44" s="3"/>
+      <c r="CS44" s="3"/>
+      <c r="CT44" s="3"/>
+      <c r="CU44" s="3"/>
+      <c r="DL44" s="3"/>
+    </row>
+    <row r="45" spans="12:116" x14ac:dyDescent="0.2">
       <c r="AI45" s="3"/>
-    </row>
-    <row r="46" spans="12:47" x14ac:dyDescent="0.2">
+      <c r="BC45" s="3"/>
+      <c r="BD45" s="3"/>
+      <c r="BE45" s="3"/>
+      <c r="BF45" s="3"/>
+      <c r="BG45" s="3"/>
+      <c r="BH45" s="3"/>
+      <c r="BI45" s="3"/>
+      <c r="BJ45" s="3"/>
+      <c r="BK45" s="3"/>
+      <c r="BL45" s="3"/>
+      <c r="BM45" s="3"/>
+      <c r="BN45" s="3"/>
+      <c r="BO45" s="3"/>
+      <c r="BP45" s="3"/>
+      <c r="BQ45" s="3"/>
+      <c r="BR45" s="3"/>
+      <c r="BS45" s="3"/>
+      <c r="BT45" s="3"/>
+      <c r="BU45" s="3"/>
+      <c r="BV45" s="3"/>
+      <c r="BW45" s="3"/>
+      <c r="BY45" s="3"/>
+      <c r="BZ45" s="3"/>
+      <c r="CA45" s="3"/>
+      <c r="CB45" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="CC45" s="24"/>
+      <c r="CD45" s="24"/>
+      <c r="CE45" s="24"/>
+      <c r="CF45" s="24"/>
+      <c r="CG45" s="3"/>
+      <c r="CH45" s="3"/>
+      <c r="CI45" s="3"/>
+      <c r="CJ45" s="3"/>
+      <c r="CK45" s="3"/>
+      <c r="CL45" s="3"/>
+      <c r="CM45" s="3"/>
+      <c r="CN45" s="3"/>
+      <c r="CO45" s="3"/>
+      <c r="CP45" s="3"/>
+      <c r="CQ45" s="3"/>
+      <c r="CR45" s="3"/>
+      <c r="CS45" s="3"/>
+      <c r="CT45" s="3"/>
+      <c r="CU45" s="3"/>
+      <c r="CV45" s="3"/>
+      <c r="CW45" s="3"/>
+      <c r="CX45" s="3"/>
+      <c r="CY45" s="3"/>
+      <c r="CZ45" s="3"/>
+      <c r="DA45" s="3"/>
+      <c r="DB45" s="3"/>
+      <c r="DC45" s="3"/>
+      <c r="DD45" s="3"/>
+      <c r="DE45" s="3"/>
+      <c r="DF45" s="3"/>
+      <c r="DG45" s="3"/>
+      <c r="DH45" s="3"/>
+      <c r="DI45" s="3"/>
+      <c r="DJ45" s="3"/>
+      <c r="DK45" s="3"/>
+      <c r="DL45" s="3"/>
+    </row>
+    <row r="46" spans="12:116" x14ac:dyDescent="0.2">
       <c r="AI46" s="3"/>
-    </row>
-    <row r="57" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BC46" s="3"/>
+      <c r="BD46" s="3"/>
+      <c r="BE46" s="3"/>
+      <c r="BF46" s="3"/>
+      <c r="BG46" s="3"/>
+      <c r="BH46" s="3"/>
+      <c r="BI46" s="3"/>
+      <c r="BJ46" s="3"/>
+      <c r="BK46" s="3"/>
+      <c r="BL46" s="3"/>
+      <c r="BM46" s="3"/>
+      <c r="BN46" s="3"/>
+      <c r="BO46" s="3"/>
+      <c r="BP46" s="3"/>
+      <c r="BQ46" s="3"/>
+      <c r="BR46" s="3"/>
+      <c r="BS46" s="3"/>
+      <c r="BY46" s="3"/>
+      <c r="BZ46" s="3"/>
+      <c r="CA46" s="3"/>
+      <c r="CB46" s="3"/>
+      <c r="CC46" s="3"/>
+      <c r="CD46" s="3"/>
+      <c r="CE46" s="3"/>
+      <c r="CP46" s="3"/>
+      <c r="DL46" s="3"/>
+    </row>
+    <row r="47" spans="12:116" x14ac:dyDescent="0.2">
+      <c r="BC47" s="3"/>
+      <c r="BD47" s="3"/>
+      <c r="BE47" s="3"/>
+      <c r="BF47" s="3"/>
+      <c r="BG47" s="3"/>
+      <c r="BH47" s="3"/>
+      <c r="BI47" s="3"/>
+      <c r="BJ47" s="3"/>
+      <c r="BK47" s="3"/>
+      <c r="BL47" s="3"/>
+      <c r="BM47" s="3"/>
+      <c r="BN47" s="3"/>
+      <c r="BO47" s="3"/>
+      <c r="BP47" s="3"/>
+      <c r="BQ47" s="3"/>
+      <c r="BR47" s="3"/>
+      <c r="BS47" s="3"/>
+      <c r="BY47" s="3"/>
+      <c r="BZ47" s="3"/>
+      <c r="CA47" s="3"/>
+      <c r="CB47" s="3"/>
+      <c r="CC47" s="3"/>
+      <c r="CD47" s="3"/>
+      <c r="CE47" s="3"/>
+      <c r="CF47" s="3"/>
+      <c r="CG47" s="3"/>
+      <c r="CH47" s="3"/>
+      <c r="CI47" s="3"/>
+      <c r="CJ47" s="3"/>
+      <c r="CK47" s="3"/>
+      <c r="CL47" s="3"/>
+      <c r="CM47" s="3"/>
+      <c r="CN47" s="3"/>
+      <c r="CO47" s="3"/>
+      <c r="CP47" s="3"/>
+      <c r="CQ47" s="3"/>
+      <c r="CR47" s="3"/>
+      <c r="CS47" s="3"/>
+      <c r="CT47" s="3"/>
+      <c r="CU47" s="3"/>
+      <c r="CV47" s="3"/>
+      <c r="CW47" s="3"/>
+      <c r="CX47" s="3"/>
+      <c r="CY47" s="3"/>
+      <c r="CZ47" s="3"/>
+      <c r="DA47" s="3"/>
+      <c r="DB47" s="3"/>
+      <c r="DC47" s="3"/>
+      <c r="DD47" s="3"/>
+      <c r="DE47" s="3"/>
+      <c r="DF47" s="3"/>
+      <c r="DG47" s="3"/>
+      <c r="DH47" s="3"/>
+      <c r="DI47" s="3"/>
+      <c r="DJ47" s="3"/>
+      <c r="DK47" s="3"/>
+      <c r="DL47" s="3"/>
+    </row>
+    <row r="48" spans="12:116" x14ac:dyDescent="0.2">
+      <c r="BC48" s="3"/>
+      <c r="BD48" s="3"/>
+      <c r="BE48" s="3"/>
+      <c r="BF48" s="3"/>
+      <c r="BG48" s="3"/>
+      <c r="BH48" s="3"/>
+      <c r="BI48" s="3"/>
+      <c r="BJ48" s="3"/>
+      <c r="BK48" s="3"/>
+      <c r="BL48" s="3"/>
+      <c r="BM48" s="3"/>
+      <c r="BN48" s="3"/>
+      <c r="BO48" s="3"/>
+      <c r="BP48" s="3"/>
+      <c r="BQ48" s="3"/>
+      <c r="BR48" s="3"/>
+      <c r="BS48" s="3"/>
+      <c r="BT48" s="3"/>
+      <c r="BU48" s="3"/>
+      <c r="BV48" s="3"/>
+      <c r="BW48" s="3"/>
+      <c r="BX48" s="3"/>
+      <c r="BY48" s="3"/>
+      <c r="BZ48" s="3"/>
+      <c r="CA48" s="3"/>
+      <c r="CB48" s="3"/>
+      <c r="CC48" s="3"/>
+      <c r="CD48" s="3"/>
+      <c r="CE48" s="3"/>
+      <c r="CP48" s="3"/>
+      <c r="DL48" s="3"/>
+    </row>
+    <row r="49" spans="6:116" x14ac:dyDescent="0.2">
+      <c r="BC49" s="3"/>
+      <c r="BD49" s="3"/>
+      <c r="BE49" s="3"/>
+      <c r="BF49" s="3"/>
+      <c r="BG49" s="3"/>
+      <c r="BH49" s="3"/>
+      <c r="BI49" s="3"/>
+      <c r="BJ49" s="3"/>
+      <c r="BK49" s="3"/>
+      <c r="BL49" s="3"/>
+      <c r="BM49" s="3"/>
+      <c r="BN49" s="3"/>
+      <c r="BO49" s="3"/>
+      <c r="BP49" s="3"/>
+      <c r="BQ49" s="3"/>
+      <c r="BR49" s="3"/>
+      <c r="BS49" s="3"/>
+      <c r="CP49" s="3"/>
+      <c r="DL49" s="3"/>
+    </row>
+    <row r="50" spans="6:116" x14ac:dyDescent="0.2">
+      <c r="BC50" s="3"/>
+      <c r="BD50" s="3"/>
+      <c r="BE50" s="3"/>
+      <c r="BF50" s="3"/>
+      <c r="BG50" s="3"/>
+      <c r="BH50" s="3"/>
+      <c r="BI50" s="3"/>
+      <c r="BJ50" s="3"/>
+      <c r="BK50" s="3"/>
+      <c r="BL50" s="3"/>
+      <c r="BM50" s="3"/>
+      <c r="BN50" s="3"/>
+      <c r="BO50" s="3"/>
+      <c r="BP50" s="3"/>
+      <c r="BQ50" s="3"/>
+      <c r="BR50" s="3"/>
+      <c r="BS50" s="3"/>
+      <c r="BT50" s="3"/>
+      <c r="BU50" s="3"/>
+      <c r="BV50" s="3"/>
+      <c r="BW50" s="3"/>
+      <c r="BX50" s="3"/>
+      <c r="BY50" s="3"/>
+      <c r="BZ50" s="3"/>
+      <c r="CA50" s="3"/>
+      <c r="CB50" s="3"/>
+      <c r="CC50" s="3"/>
+      <c r="CD50" s="3"/>
+      <c r="CE50" s="3"/>
+      <c r="CF50" s="3"/>
+      <c r="CG50" s="3"/>
+      <c r="CH50" s="3"/>
+      <c r="CI50" s="3"/>
+      <c r="CJ50" s="3"/>
+      <c r="CK50" s="3"/>
+      <c r="CL50" s="3"/>
+      <c r="CM50" s="3"/>
+      <c r="CN50" s="3"/>
+      <c r="CO50" s="3"/>
+      <c r="CP50" s="3"/>
+      <c r="CQ50" s="3"/>
+      <c r="CR50" s="3"/>
+      <c r="CS50" s="3"/>
+      <c r="CT50" s="3"/>
+      <c r="CU50" s="3"/>
+      <c r="CV50" s="3"/>
+      <c r="CW50" s="3"/>
+      <c r="CX50" s="3"/>
+      <c r="CY50" s="3"/>
+      <c r="CZ50" s="3"/>
+      <c r="DA50" s="3"/>
+      <c r="DB50" s="3"/>
+      <c r="DC50" s="3"/>
+      <c r="DD50" s="3"/>
+      <c r="DE50" s="3"/>
+      <c r="DF50" s="3"/>
+      <c r="DG50" s="3"/>
+      <c r="DH50" s="3"/>
+      <c r="DI50" s="3"/>
+      <c r="DJ50" s="3"/>
+      <c r="DK50" s="3"/>
+      <c r="DL50" s="3"/>
+    </row>
+    <row r="51" spans="6:116" x14ac:dyDescent="0.2">
+      <c r="BC51" s="3"/>
+      <c r="BD51" s="3"/>
+      <c r="BE51" s="3"/>
+      <c r="BF51" s="3"/>
+      <c r="BG51" s="3"/>
+      <c r="BH51" s="3"/>
+      <c r="BI51" s="3"/>
+      <c r="BJ51" s="3"/>
+      <c r="BK51" s="3"/>
+      <c r="BL51" s="3"/>
+      <c r="BM51" s="3"/>
+      <c r="BN51" s="3"/>
+      <c r="BO51" s="3"/>
+      <c r="BP51" s="3"/>
+      <c r="BQ51" s="3"/>
+      <c r="BR51" s="3"/>
+      <c r="BS51" s="3"/>
+      <c r="CE51" s="3"/>
+      <c r="CF51" s="3"/>
+      <c r="CG51" s="3"/>
+      <c r="CH51" s="3"/>
+      <c r="CI51" s="3"/>
+      <c r="CJ51" s="3"/>
+      <c r="CK51" s="3"/>
+      <c r="CL51" s="3"/>
+      <c r="CM51" s="3"/>
+      <c r="CN51" s="3"/>
+      <c r="CO51" s="3"/>
+      <c r="CP51" s="3"/>
+      <c r="CQ51" s="3"/>
+      <c r="CR51" s="3"/>
+      <c r="CS51" s="3"/>
+      <c r="CT51" s="3"/>
+      <c r="CU51" s="3"/>
+    </row>
+    <row r="52" spans="6:116" x14ac:dyDescent="0.2">
+      <c r="BC52" s="3"/>
+      <c r="BD52" s="3"/>
+      <c r="BE52" s="3"/>
+      <c r="BF52" s="3"/>
+      <c r="BG52" s="3"/>
+      <c r="BH52" s="3"/>
+      <c r="BI52" s="3"/>
+      <c r="BJ52" s="3"/>
+      <c r="BK52" s="3"/>
+      <c r="BL52" s="3"/>
+      <c r="BM52" s="3"/>
+      <c r="BN52" s="3"/>
+      <c r="BO52" s="3"/>
+      <c r="BP52" s="3"/>
+      <c r="BQ52" s="3"/>
+      <c r="BR52" s="3"/>
+      <c r="BS52" s="3"/>
+      <c r="CE52" s="20"/>
+      <c r="CF52" s="20"/>
+      <c r="CG52" s="20"/>
+      <c r="CH52" s="20"/>
+      <c r="CI52" s="20"/>
+      <c r="CJ52" s="20"/>
+      <c r="CK52" s="20"/>
+      <c r="CL52" s="20"/>
+      <c r="CM52" s="20"/>
+      <c r="CN52" s="20"/>
+      <c r="CO52" s="20"/>
+      <c r="CP52" s="20"/>
+      <c r="CQ52" s="20"/>
+      <c r="CR52" s="20"/>
+      <c r="CS52" s="20"/>
+      <c r="CT52" s="20"/>
+      <c r="CU52" s="20"/>
+    </row>
+    <row r="53" spans="6:116" x14ac:dyDescent="0.2">
+      <c r="BC53" s="3"/>
+      <c r="BD53" s="3"/>
+      <c r="BE53" s="3"/>
+      <c r="BF53" s="3"/>
+      <c r="BG53" s="3"/>
+      <c r="BH53" s="3"/>
+      <c r="BI53" s="3"/>
+      <c r="BJ53" s="3"/>
+      <c r="BK53" s="3"/>
+      <c r="BL53" s="3"/>
+      <c r="BM53" s="3"/>
+      <c r="BN53" s="3"/>
+      <c r="BO53" s="3"/>
+      <c r="BP53" s="3"/>
+      <c r="BQ53" s="3"/>
+      <c r="BR53" s="3"/>
+      <c r="BS53" s="3"/>
+      <c r="CE53" s="3"/>
+      <c r="CF53" s="3"/>
+      <c r="CG53" s="3"/>
+      <c r="CH53" s="3"/>
+      <c r="CI53" s="3"/>
+      <c r="CJ53" s="3"/>
+      <c r="CK53" s="3"/>
+      <c r="CL53" s="3"/>
+      <c r="CM53" s="3"/>
+      <c r="CN53" s="3"/>
+      <c r="CO53" s="3"/>
+      <c r="CP53" s="3"/>
+      <c r="CQ53" s="3"/>
+      <c r="CR53" s="3"/>
+      <c r="CS53" s="3"/>
+      <c r="CT53" s="3"/>
+      <c r="CU53" s="3"/>
+    </row>
+    <row r="54" spans="6:116" x14ac:dyDescent="0.2">
+      <c r="BC54" s="3"/>
+      <c r="BD54" s="3"/>
+      <c r="BE54" s="3"/>
+      <c r="BF54" s="3"/>
+      <c r="BG54" s="3"/>
+      <c r="BH54" s="3"/>
+      <c r="BI54" s="3"/>
+      <c r="BJ54" s="3"/>
+      <c r="BK54" s="3"/>
+      <c r="BL54" s="3"/>
+      <c r="BM54" s="3"/>
+      <c r="BN54" s="3"/>
+      <c r="BO54" s="3"/>
+      <c r="BP54" s="3"/>
+      <c r="BQ54" s="3"/>
+      <c r="BR54" s="3"/>
+      <c r="BS54" s="3"/>
+      <c r="CE54" s="3"/>
+      <c r="CF54" s="3"/>
+      <c r="CG54" s="3"/>
+      <c r="CH54" s="3"/>
+      <c r="CI54" s="3"/>
+      <c r="CJ54" s="3"/>
+      <c r="CK54" s="3"/>
+      <c r="CL54" s="3"/>
+      <c r="CM54" s="3"/>
+      <c r="CN54" s="3"/>
+      <c r="CO54" s="3"/>
+      <c r="CP54" s="3"/>
+      <c r="CQ54" s="3"/>
+      <c r="CR54" s="3"/>
+      <c r="CS54" s="3"/>
+      <c r="CT54" s="3"/>
+      <c r="CU54" s="3"/>
+    </row>
+    <row r="57" spans="6:116" x14ac:dyDescent="0.2">
       <c r="Z57" s="3"/>
       <c r="AA57" s="3"/>
       <c r="AB57" s="3"/>
@@ -1260,7 +2595,7 @@
       <c r="AD57" s="3"/>
       <c r="AE57" s="3"/>
     </row>
-    <row r="58" spans="6:76" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:116" x14ac:dyDescent="0.2">
       <c r="Z58" s="3"/>
       <c r="AA58" s="3"/>
       <c r="AB58" s="3"/>
@@ -1268,7 +2603,7 @@
       <c r="AD58" s="3"/>
       <c r="AE58" s="3"/>
     </row>
-    <row r="59" spans="6:76" x14ac:dyDescent="0.2">
+    <row r="59" spans="6:116" x14ac:dyDescent="0.2">
       <c r="Z59" s="3"/>
       <c r="AA59" s="3"/>
       <c r="AB59" s="3"/>
@@ -1276,7 +2611,7 @@
       <c r="AD59" s="3"/>
       <c r="AE59" s="3"/>
     </row>
-    <row r="60" spans="6:76" x14ac:dyDescent="0.2">
+    <row r="60" spans="6:116" x14ac:dyDescent="0.2">
       <c r="Z60" s="3"/>
       <c r="AA60" s="3"/>
       <c r="AB60" s="3"/>
@@ -1284,7 +2619,7 @@
       <c r="AD60" s="3"/>
       <c r="AE60" s="3"/>
     </row>
-    <row r="61" spans="6:76" x14ac:dyDescent="0.2">
+    <row r="61" spans="6:116" x14ac:dyDescent="0.2">
       <c r="Z61" s="3"/>
       <c r="AA61" s="3"/>
       <c r="AB61" s="3"/>
@@ -1299,7 +2634,7 @@
       <c r="BW61" s="3"/>
       <c r="BX61" s="3"/>
     </row>
-    <row r="62" spans="6:76" x14ac:dyDescent="0.2">
+    <row r="62" spans="6:116" x14ac:dyDescent="0.2">
       <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
       <c r="AA62" s="3"/>
@@ -1323,7 +2658,7 @@
       <c r="BW62" s="3"/>
       <c r="BX62" s="3"/>
     </row>
-    <row r="63" spans="6:76" x14ac:dyDescent="0.2">
+    <row r="63" spans="6:116" x14ac:dyDescent="0.2">
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -1351,7 +2686,7 @@
       <c r="BW63" s="3"/>
       <c r="BX63" s="3"/>
     </row>
-    <row r="64" spans="6:76" x14ac:dyDescent="0.2">
+    <row r="64" spans="6:116" x14ac:dyDescent="0.2">
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -1669,8 +3004,8 @@
       <c r="AY70" s="3"/>
       <c r="AZ70" s="3"/>
       <c r="BA70" s="3"/>
-      <c r="BC70" s="17"/>
-      <c r="BD70" s="17"/>
+      <c r="BC70" s="16"/>
+      <c r="BD70" s="16"/>
       <c r="BE70" s="3"/>
       <c r="BF70" s="3"/>
       <c r="BG70" s="3"/>
@@ -1714,8 +3049,8 @@
       <c r="AY71" s="3"/>
       <c r="AZ71" s="3"/>
       <c r="BA71" s="3"/>
-      <c r="BC71" s="17"/>
-      <c r="BD71" s="17"/>
+      <c r="BC71" s="16"/>
+      <c r="BD71" s="16"/>
       <c r="BE71" s="3"/>
       <c r="BF71" s="3"/>
       <c r="BG71" s="3"/>
@@ -1792,10 +3127,10 @@
       <c r="BG72" s="10"/>
       <c r="BH72" s="10"/>
       <c r="BI72" s="10"/>
-      <c r="BJ72" s="18"/>
-      <c r="BK72" s="18"/>
-      <c r="BL72" s="18"/>
-      <c r="BM72" s="19"/>
+      <c r="BJ72" s="17"/>
+      <c r="BK72" s="17"/>
+      <c r="BL72" s="17"/>
+      <c r="BM72" s="18"/>
       <c r="BN72" s="10"/>
       <c r="BO72" s="10"/>
       <c r="BP72" s="10"/>
@@ -2024,14 +3359,14 @@
       <c r="BU77" s="10"/>
     </row>
     <row r="78" spans="6:78" x14ac:dyDescent="0.2">
-      <c r="M78" s="16"/>
-      <c r="N78" s="16"/>
-      <c r="O78" s="16"/>
-      <c r="P78" s="16"/>
-      <c r="Q78" s="16"/>
-      <c r="R78" s="16"/>
-      <c r="S78" s="16"/>
-      <c r="T78" s="16"/>
+      <c r="M78" s="21"/>
+      <c r="N78" s="21"/>
+      <c r="O78" s="21"/>
+      <c r="P78" s="21"/>
+      <c r="Q78" s="21"/>
+      <c r="R78" s="21"/>
+      <c r="S78" s="21"/>
+      <c r="T78" s="21"/>
       <c r="AN78" s="3"/>
       <c r="AO78" s="3"/>
       <c r="AP78" s="3"/>
@@ -2884,20 +4219,20 @@
       <c r="AR105" s="3"/>
       <c r="AS105" s="3"/>
       <c r="AT105" s="3"/>
-      <c r="AU105" s="21"/>
-      <c r="AV105" s="21"/>
-      <c r="AW105" s="21"/>
-      <c r="AX105" s="21"/>
-      <c r="AY105" s="21"/>
-      <c r="AZ105" s="21"/>
-      <c r="BA105" s="21"/>
-      <c r="BB105" s="21"/>
-      <c r="BC105" s="21"/>
-      <c r="BD105" s="21"/>
-      <c r="BE105" s="21"/>
-      <c r="BF105" s="21"/>
-      <c r="BG105" s="21"/>
-      <c r="BH105" s="21"/>
+      <c r="AU105" s="20"/>
+      <c r="AV105" s="20"/>
+      <c r="AW105" s="20"/>
+      <c r="AX105" s="20"/>
+      <c r="AY105" s="20"/>
+      <c r="AZ105" s="20"/>
+      <c r="BA105" s="20"/>
+      <c r="BB105" s="20"/>
+      <c r="BC105" s="20"/>
+      <c r="BD105" s="20"/>
+      <c r="BE105" s="20"/>
+      <c r="BF105" s="20"/>
+      <c r="BG105" s="20"/>
+      <c r="BH105" s="20"/>
       <c r="BI105" s="3"/>
       <c r="BJ105" s="3"/>
       <c r="BK105" s="3"/>
@@ -2955,20 +4290,20 @@
       <c r="AR106" s="3"/>
       <c r="AS106" s="3"/>
       <c r="AT106" s="3"/>
-      <c r="AU106" s="21"/>
-      <c r="AV106" s="21"/>
-      <c r="AW106" s="21"/>
-      <c r="AX106" s="21"/>
-      <c r="AY106" s="21"/>
-      <c r="AZ106" s="21"/>
-      <c r="BA106" s="21"/>
-      <c r="BB106" s="21"/>
-      <c r="BC106" s="21"/>
-      <c r="BD106" s="21"/>
-      <c r="BE106" s="21"/>
-      <c r="BF106" s="21"/>
-      <c r="BG106" s="21"/>
-      <c r="BH106" s="21"/>
+      <c r="AU106" s="20"/>
+      <c r="AV106" s="20"/>
+      <c r="AW106" s="20"/>
+      <c r="AX106" s="20"/>
+      <c r="AY106" s="20"/>
+      <c r="AZ106" s="20"/>
+      <c r="BA106" s="20"/>
+      <c r="BB106" s="20"/>
+      <c r="BC106" s="20"/>
+      <c r="BD106" s="20"/>
+      <c r="BE106" s="20"/>
+      <c r="BF106" s="20"/>
+      <c r="BG106" s="20"/>
+      <c r="BH106" s="20"/>
       <c r="BI106" s="3"/>
       <c r="BJ106" s="3"/>
       <c r="BK106" s="3"/>
@@ -3015,20 +4350,20 @@
       <c r="AI107" s="3"/>
       <c r="AJ107" s="3"/>
       <c r="AK107" s="3"/>
-      <c r="AU107" s="21"/>
-      <c r="AV107" s="21"/>
-      <c r="AW107" s="21"/>
-      <c r="AX107" s="21"/>
-      <c r="AY107" s="21"/>
-      <c r="AZ107" s="21"/>
-      <c r="BA107" s="21"/>
-      <c r="BB107" s="21"/>
-      <c r="BC107" s="21"/>
-      <c r="BD107" s="21"/>
-      <c r="BE107" s="21"/>
-      <c r="BF107" s="21"/>
-      <c r="BG107" s="21"/>
-      <c r="BH107" s="21"/>
+      <c r="AU107" s="20"/>
+      <c r="AV107" s="20"/>
+      <c r="AW107" s="20"/>
+      <c r="AX107" s="20"/>
+      <c r="AY107" s="20"/>
+      <c r="AZ107" s="20"/>
+      <c r="BA107" s="20"/>
+      <c r="BB107" s="20"/>
+      <c r="BC107" s="20"/>
+      <c r="BD107" s="20"/>
+      <c r="BE107" s="20"/>
+      <c r="BF107" s="20"/>
+      <c r="BG107" s="20"/>
+      <c r="BH107" s="20"/>
       <c r="BL107" s="3"/>
       <c r="BP107" s="3"/>
       <c r="BQ107" s="3"/>
@@ -3062,20 +4397,20 @@
       <c r="AI108" s="3"/>
       <c r="AJ108" s="3"/>
       <c r="AK108" s="3"/>
-      <c r="AU108" s="21"/>
-      <c r="AV108" s="21"/>
-      <c r="AW108" s="21"/>
-      <c r="AX108" s="21"/>
-      <c r="AY108" s="21"/>
-      <c r="AZ108" s="21"/>
-      <c r="BA108" s="21"/>
-      <c r="BB108" s="21"/>
-      <c r="BC108" s="21"/>
-      <c r="BD108" s="21"/>
-      <c r="BE108" s="21"/>
-      <c r="BF108" s="21"/>
-      <c r="BG108" s="21"/>
-      <c r="BH108" s="21"/>
+      <c r="AU108" s="20"/>
+      <c r="AV108" s="20"/>
+      <c r="AW108" s="20"/>
+      <c r="AX108" s="20"/>
+      <c r="AY108" s="20"/>
+      <c r="AZ108" s="20"/>
+      <c r="BA108" s="20"/>
+      <c r="BB108" s="20"/>
+      <c r="BC108" s="20"/>
+      <c r="BD108" s="20"/>
+      <c r="BE108" s="20"/>
+      <c r="BF108" s="20"/>
+      <c r="BG108" s="20"/>
+      <c r="BH108" s="20"/>
       <c r="BI108" s="3"/>
       <c r="BJ108" s="3"/>
       <c r="BK108" s="3"/>
@@ -3110,20 +4445,20 @@
     <row r="109" spans="24:93" x14ac:dyDescent="0.2">
       <c r="AJ109" s="3"/>
       <c r="AK109" s="3"/>
-      <c r="AU109" s="21"/>
-      <c r="AV109" s="21"/>
-      <c r="AW109" s="21"/>
-      <c r="AX109" s="21"/>
-      <c r="AY109" s="21"/>
-      <c r="AZ109" s="21"/>
-      <c r="BA109" s="21"/>
-      <c r="BB109" s="21"/>
-      <c r="BC109" s="21"/>
-      <c r="BD109" s="21"/>
-      <c r="BE109" s="21"/>
-      <c r="BF109" s="21"/>
-      <c r="BG109" s="21"/>
-      <c r="BH109" s="21"/>
+      <c r="AU109" s="20"/>
+      <c r="AV109" s="20"/>
+      <c r="AW109" s="20"/>
+      <c r="AX109" s="20"/>
+      <c r="AY109" s="20"/>
+      <c r="AZ109" s="20"/>
+      <c r="BA109" s="20"/>
+      <c r="BB109" s="20"/>
+      <c r="BC109" s="20"/>
+      <c r="BD109" s="20"/>
+      <c r="BE109" s="20"/>
+      <c r="BF109" s="20"/>
+      <c r="BG109" s="20"/>
+      <c r="BH109" s="20"/>
       <c r="BI109" s="3"/>
       <c r="BJ109" s="3"/>
       <c r="BK109" s="3"/>
@@ -3158,20 +4493,20 @@
     <row r="110" spans="24:93" x14ac:dyDescent="0.2">
       <c r="AJ110" s="3"/>
       <c r="AK110" s="3"/>
-      <c r="AU110" s="21"/>
-      <c r="AV110" s="21"/>
-      <c r="AW110" s="21"/>
-      <c r="AX110" s="21"/>
-      <c r="AY110" s="21"/>
-      <c r="AZ110" s="21"/>
-      <c r="BA110" s="21"/>
-      <c r="BB110" s="21"/>
-      <c r="BC110" s="21"/>
-      <c r="BD110" s="21"/>
-      <c r="BE110" s="21"/>
-      <c r="BF110" s="21"/>
-      <c r="BG110" s="21"/>
-      <c r="BH110" s="21"/>
+      <c r="AU110" s="20"/>
+      <c r="AV110" s="20"/>
+      <c r="AW110" s="20"/>
+      <c r="AX110" s="20"/>
+      <c r="AY110" s="20"/>
+      <c r="AZ110" s="20"/>
+      <c r="BA110" s="20"/>
+      <c r="BB110" s="20"/>
+      <c r="BC110" s="20"/>
+      <c r="BD110" s="20"/>
+      <c r="BE110" s="20"/>
+      <c r="BF110" s="20"/>
+      <c r="BG110" s="20"/>
+      <c r="BH110" s="20"/>
       <c r="BI110" s="3"/>
       <c r="BJ110" s="3"/>
       <c r="BK110" s="14"/>
@@ -3203,28 +4538,28 @@
       <c r="CN110" s="3"/>
     </row>
     <row r="111" spans="24:93" x14ac:dyDescent="0.2">
-      <c r="AE111" s="16"/>
-      <c r="AF111" s="16"/>
-      <c r="AG111" s="16"/>
-      <c r="AH111" s="16"/>
-      <c r="AI111" s="16"/>
-      <c r="AJ111" s="16"/>
-      <c r="AK111" s="16"/>
-      <c r="AL111" s="16"/>
-      <c r="AU111" s="21"/>
-      <c r="AV111" s="21"/>
-      <c r="AW111" s="21"/>
-      <c r="AX111" s="21"/>
-      <c r="AY111" s="21"/>
-      <c r="AZ111" s="21"/>
-      <c r="BA111" s="21"/>
-      <c r="BB111" s="21"/>
-      <c r="BC111" s="21"/>
-      <c r="BD111" s="21"/>
-      <c r="BE111" s="21"/>
-      <c r="BF111" s="21"/>
-      <c r="BG111" s="21"/>
-      <c r="BH111" s="21"/>
+      <c r="AE111" s="21"/>
+      <c r="AF111" s="21"/>
+      <c r="AG111" s="21"/>
+      <c r="AH111" s="21"/>
+      <c r="AI111" s="21"/>
+      <c r="AJ111" s="21"/>
+      <c r="AK111" s="21"/>
+      <c r="AL111" s="21"/>
+      <c r="AU111" s="20"/>
+      <c r="AV111" s="20"/>
+      <c r="AW111" s="20"/>
+      <c r="AX111" s="20"/>
+      <c r="AY111" s="20"/>
+      <c r="AZ111" s="20"/>
+      <c r="BA111" s="20"/>
+      <c r="BB111" s="20"/>
+      <c r="BC111" s="20"/>
+      <c r="BD111" s="20"/>
+      <c r="BE111" s="20"/>
+      <c r="BF111" s="20"/>
+      <c r="BG111" s="20"/>
+      <c r="BH111" s="20"/>
       <c r="BI111" s="3"/>
       <c r="BJ111" s="3"/>
       <c r="BK111" s="14"/>
@@ -3257,20 +4592,20 @@
     </row>
     <row r="112" spans="24:93" x14ac:dyDescent="0.2">
       <c r="AJ112" s="3"/>
-      <c r="AU112" s="21"/>
-      <c r="AV112" s="21"/>
-      <c r="AW112" s="21"/>
-      <c r="AX112" s="21"/>
-      <c r="AY112" s="21"/>
-      <c r="AZ112" s="21"/>
-      <c r="BA112" s="21"/>
-      <c r="BB112" s="21"/>
-      <c r="BC112" s="21"/>
-      <c r="BD112" s="21"/>
-      <c r="BE112" s="21"/>
-      <c r="BF112" s="21"/>
-      <c r="BG112" s="21"/>
-      <c r="BH112" s="21"/>
+      <c r="AU112" s="20"/>
+      <c r="AV112" s="20"/>
+      <c r="AW112" s="20"/>
+      <c r="AX112" s="20"/>
+      <c r="AY112" s="20"/>
+      <c r="AZ112" s="20"/>
+      <c r="BA112" s="20"/>
+      <c r="BB112" s="20"/>
+      <c r="BC112" s="20"/>
+      <c r="BD112" s="20"/>
+      <c r="BE112" s="20"/>
+      <c r="BF112" s="20"/>
+      <c r="BG112" s="20"/>
+      <c r="BH112" s="20"/>
       <c r="BI112" s="3"/>
       <c r="BJ112" s="3"/>
       <c r="BK112" s="14"/>
@@ -3300,20 +4635,20 @@
     </row>
     <row r="113" spans="26:93" x14ac:dyDescent="0.2">
       <c r="AJ113" s="3"/>
-      <c r="AU113" s="21"/>
-      <c r="AV113" s="21"/>
-      <c r="AW113" s="21"/>
-      <c r="AX113" s="21"/>
-      <c r="AY113" s="21"/>
-      <c r="AZ113" s="21"/>
-      <c r="BA113" s="21"/>
-      <c r="BB113" s="21"/>
-      <c r="BC113" s="21"/>
-      <c r="BD113" s="21"/>
-      <c r="BE113" s="21"/>
-      <c r="BF113" s="21"/>
-      <c r="BG113" s="21"/>
-      <c r="BH113" s="21"/>
+      <c r="AU113" s="20"/>
+      <c r="AV113" s="20"/>
+      <c r="AW113" s="20"/>
+      <c r="AX113" s="20"/>
+      <c r="AY113" s="20"/>
+      <c r="AZ113" s="20"/>
+      <c r="BA113" s="20"/>
+      <c r="BB113" s="20"/>
+      <c r="BC113" s="20"/>
+      <c r="BD113" s="20"/>
+      <c r="BE113" s="20"/>
+      <c r="BF113" s="20"/>
+      <c r="BG113" s="20"/>
+      <c r="BH113" s="20"/>
       <c r="BI113" s="3"/>
       <c r="BJ113" s="3"/>
       <c r="BL113" s="3"/>
@@ -3468,16 +4803,16 @@
       <c r="CO116" s="3"/>
     </row>
     <row r="117" spans="26:93" x14ac:dyDescent="0.2">
-      <c r="AI117" s="16"/>
-      <c r="AJ117" s="16"/>
-      <c r="AK117" s="16"/>
-      <c r="AL117" s="16"/>
-      <c r="AM117" s="16"/>
-      <c r="AN117" s="16"/>
-      <c r="AO117" s="16"/>
-      <c r="AP117" s="16"/>
-      <c r="AQ117" s="16"/>
-      <c r="AR117" s="20"/>
+      <c r="AI117" s="21"/>
+      <c r="AJ117" s="21"/>
+      <c r="AK117" s="21"/>
+      <c r="AL117" s="21"/>
+      <c r="AM117" s="21"/>
+      <c r="AN117" s="21"/>
+      <c r="AO117" s="21"/>
+      <c r="AP117" s="21"/>
+      <c r="AQ117" s="21"/>
+      <c r="AR117" s="19"/>
       <c r="AS117" s="3"/>
       <c r="AT117" s="3"/>
       <c r="AU117" s="3"/>
@@ -3516,16 +4851,16 @@
       <c r="CO117" s="3"/>
     </row>
     <row r="118" spans="26:93" x14ac:dyDescent="0.2">
-      <c r="AI118" s="16"/>
-      <c r="AJ118" s="16"/>
-      <c r="AK118" s="16"/>
-      <c r="AL118" s="16"/>
-      <c r="AM118" s="16"/>
-      <c r="AN118" s="16"/>
-      <c r="AO118" s="16"/>
-      <c r="AP118" s="16"/>
-      <c r="AQ118" s="16"/>
-      <c r="AR118" s="20"/>
+      <c r="AI118" s="21"/>
+      <c r="AJ118" s="21"/>
+      <c r="AK118" s="21"/>
+      <c r="AL118" s="21"/>
+      <c r="AM118" s="21"/>
+      <c r="AN118" s="21"/>
+      <c r="AO118" s="21"/>
+      <c r="AP118" s="21"/>
+      <c r="AQ118" s="21"/>
+      <c r="AR118" s="19"/>
       <c r="AS118" s="3"/>
       <c r="AT118" s="3"/>
       <c r="AU118" s="3"/>
@@ -3582,15 +4917,15 @@
       <c r="AC119" s="7"/>
       <c r="AD119" s="7"/>
       <c r="AE119" s="7"/>
-      <c r="AI119" s="16"/>
-      <c r="AJ119" s="16"/>
-      <c r="AK119" s="16"/>
-      <c r="AL119" s="16"/>
-      <c r="AM119" s="16"/>
-      <c r="AN119" s="16"/>
-      <c r="AO119" s="16"/>
-      <c r="AP119" s="16"/>
-      <c r="AQ119" s="16"/>
+      <c r="AI119" s="21"/>
+      <c r="AJ119" s="21"/>
+      <c r="AK119" s="21"/>
+      <c r="AL119" s="21"/>
+      <c r="AM119" s="21"/>
+      <c r="AN119" s="21"/>
+      <c r="AO119" s="21"/>
+      <c r="AP119" s="21"/>
+      <c r="AQ119" s="21"/>
       <c r="AR119" s="3"/>
       <c r="AS119" s="3"/>
       <c r="AT119" s="3"/>
@@ -3661,7 +4996,7 @@
       <c r="BT120" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="AI119:AQ119"/>
     <mergeCell ref="M78:T78"/>
     <mergeCell ref="AE111:AL111"/>
@@ -3672,6 +5007,8 @@
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="F5:J5"/>
+    <mergeCell ref="CB44:CF44"/>
+    <mergeCell ref="CB45:CF45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>